<commit_message>
HREOS-11546 - Rellenar excel
</commit_message>
<xml_diff>
--- a/rem-web/src/main/webapp/plantillas/plugin/GenerarFichaComercialBbva/FichaComercialReport.xlsx
+++ b/rem-web/src/main/webapp/plantillas/plugin/GenerarFichaComercialBbva/FichaComercialReport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Oferta BBVA" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="146">
   <si>
     <t xml:space="preserve">ID OFERTA:</t>
   </si>
@@ -550,9 +550,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Este cuadro saldrá vacío para que el GM lo rellene</t>
-  </si>
-  <si>
     <t xml:space="preserve">para que, mancomunadamente, dos cualesquiera de ellos, puedan llevar a cabo las facultades que las escrituras que se referencian en el Anexo III les confieren, en relación con la transmisión de los inmuebles cuyos datos se describen a continuación y en los términos y condiciones que figuran en el presente documento:</t>
   </si>
   <si>
@@ -569,9 +566,6 @@
   </si>
   <si>
     <t xml:space="preserve">Otras condiciones de la venta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saldrá una línea por activo de la oferta</t>
   </si>
   <si>
     <t xml:space="preserve">Se hace constar que los Apoderados lo son de la entidad HAYA REAL ESTATE, S.A.U., con domicilio social en Madrid, Medina de Pomar 27, con C.I.F.-A86744349 e inscrita en el Registro Mercantil de Madrid, en la Hoja M-550663, a quien las apoderantes confirieron los correspondientes poderes que se incluyen en el Anexo IV.</t>
@@ -597,19 +591,19 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00&quot; €&quot;_-;\-* #,##0.00&quot; €&quot;_-;_-* \-??&quot; €&quot;_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="167" formatCode="#,##0"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0&quot; €&quot;_-;\-* #,##0&quot; €&quot;_-;_-* &quot;- €&quot;_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="General"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0&quot; €&quot;_-;\-* #,##0&quot; €&quot;_-;_-* \-??&quot; €&quot;_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="0.00\ %"/>
-    <numFmt numFmtId="172" formatCode="#,##0.00&quot; m²&quot;"/>
-    <numFmt numFmtId="173" formatCode="0\ %"/>
-    <numFmt numFmtId="174" formatCode="#,##0.00"/>
-    <numFmt numFmtId="175" formatCode="#"/>
-    <numFmt numFmtId="176" formatCode="###,###,###"/>
-    <numFmt numFmtId="177" formatCode="@"/>
+    <numFmt numFmtId="167" formatCode="@"/>
+    <numFmt numFmtId="168" formatCode="#,##0"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0&quot; €&quot;_-;\-* #,##0&quot; €&quot;_-;_-* &quot;- €&quot;_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="General"/>
+    <numFmt numFmtId="171" formatCode="_-* #,##0&quot; €&quot;_-;\-* #,##0&quot; €&quot;_-;_-* \-??&quot; €&quot;_-;_-@_-"/>
+    <numFmt numFmtId="172" formatCode="0.00\ %"/>
+    <numFmt numFmtId="173" formatCode="#,##0.00&quot; m²&quot;"/>
+    <numFmt numFmtId="174" formatCode="0\ %"/>
+    <numFmt numFmtId="175" formatCode="#,##0.00"/>
+    <numFmt numFmtId="176" formatCode="#"/>
+    <numFmt numFmtId="177" formatCode="###,###,###"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -686,7 +680,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
       <sz val="8"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
@@ -696,6 +689,14 @@
     <font>
       <b val="true"/>
       <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1119,20 +1120,20 @@
       <left/>
       <right/>
       <top style="thin">
-        <color rgb="FFD9D9D9"/>
+        <color rgb="FFA5A5A5"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFD9D9D9"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top style="thin">
-        <color rgb="FFA5A5A5"/>
+        <color rgb="FFD9D9D9"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FFD9D9D9"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -1183,7 +1184,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="143">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1229,7 +1230,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1252,8 +1253,8 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1281,49 +1282,53 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="168" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="169" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1368,19 +1373,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="13" fillId="0" borderId="16" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="14" fillId="0" borderId="16" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="15" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="17" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="15" fillId="0" borderId="17" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1388,11 +1393,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
@@ -1400,7 +1405,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="13" fillId="0" borderId="18" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="14" fillId="0" borderId="18" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1408,39 +1413,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="13" fillId="0" borderId="20" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="14" fillId="0" borderId="20" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="11" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="15" fillId="0" borderId="11" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="14" fillId="0" borderId="19" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="15" fillId="0" borderId="19" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="13" fillId="0" borderId="21" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="14" fillId="0" borderId="21" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="16" fillId="0" borderId="23" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="17" fillId="0" borderId="23" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="173" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="18" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="18" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="16" fillId="0" borderId="24" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="17" fillId="0" borderId="24" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1468,13 +1473,9 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -1484,7 +1485,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
@@ -1524,7 +1525,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="174" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1544,7 +1545,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="17" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="18" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1552,119 +1553,95 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="173" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="9" fillId="7" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="9" fillId="7" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="174" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="175" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="8" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="8" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="8" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="8" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="8" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="28" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="174" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="28" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="27" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="28" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="4" fillId="2" borderId="28" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="4" fillId="3" borderId="28" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="8" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1672,7 +1649,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1684,95 +1661,99 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="10" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="10" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
     <xf numFmtId="164" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="11" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="11" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="11" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="11" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="175" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="176" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="176" fontId="25" fillId="0" borderId="14" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="177" fontId="26" fillId="0" borderId="14" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1883,9 +1864,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1504800</xdr:colOff>
+      <xdr:colOff>1503720</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>156240</xdr:rowOff>
+      <xdr:rowOff>155160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1900,7 +1881,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="533520" y="190440"/>
-          <a:ext cx="1504440" cy="506520"/>
+          <a:ext cx="1503360" cy="505440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1926,9 +1907,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1129680</xdr:colOff>
+      <xdr:colOff>1128600</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>122400</xdr:rowOff>
+      <xdr:rowOff>121320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1943,7 +1924,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="279360" y="190440"/>
-          <a:ext cx="1993320" cy="503280"/>
+          <a:ext cx="1990800" cy="502200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1969,9 +1950,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>38160</xdr:colOff>
+      <xdr:colOff>37080</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>125640</xdr:rowOff>
+      <xdr:rowOff>124560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1986,7 +1967,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="254160" y="190440"/>
-          <a:ext cx="1911240" cy="506520"/>
+          <a:ext cx="1911240" cy="505440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2012,9 +1993,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>19080</xdr:colOff>
+      <xdr:colOff>18000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>125640</xdr:rowOff>
+      <xdr:rowOff>124560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2029,7 +2010,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="317520" y="190440"/>
-          <a:ext cx="1892160" cy="506520"/>
+          <a:ext cx="1892160" cy="505440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2091,11 +2072,11 @@
   </sheetPr>
   <dimension ref="B2:M74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C58" activeCellId="0" sqref="C58"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.14"/>
@@ -2322,6 +2303,7 @@
       <c r="L24" s="34"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="35"/>
       <c r="H25" s="34"/>
       <c r="I25" s="34"/>
       <c r="J25" s="34"/>
@@ -2355,235 +2337,235 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C30" s="35" t="s">
+      <c r="C30" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="36"/>
-      <c r="E30" s="37" t="s">
+      <c r="D30" s="37"/>
+      <c r="E30" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="F30" s="38" t="s">
+      <c r="F30" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
       <c r="M30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="39"/>
-      <c r="D31" s="40" t="s">
+      <c r="C31" s="40"/>
+      <c r="D31" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="41"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="J31" s="44" t="s">
+      <c r="E31" s="42"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="44"/>
+      <c r="J31" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="K31" s="43" t="s">
+      <c r="K31" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="L31" s="43" t="s">
+      <c r="L31" s="44" t="s">
         <v>33</v>
       </c>
       <c r="M31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="45" t="s">
+      <c r="C32" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="46" t="str">
+      <c r="D32" s="47" t="str">
         <f aca="false">IF(E32&gt;0,CONCATENATE(ROUND((((E39/E32)-1)*100),2)," %"),"")</f>
         <v/>
       </c>
-      <c r="E32" s="47"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="49"/>
-      <c r="J32" s="50"/>
-      <c r="K32" s="51"/>
-      <c r="L32" s="52"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="50"/>
+      <c r="J32" s="51"/>
+      <c r="K32" s="52"/>
+      <c r="L32" s="53"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="53" t="s">
+      <c r="C33" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="46" t="str">
+      <c r="D33" s="47" t="str">
         <f aca="false">IF(E33&gt;0,CONCATENATE(ROUND((((E39/E33)-1)*100),2)," %"),"")</f>
         <v/>
       </c>
-      <c r="E33" s="54"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="50"/>
+      <c r="H33" s="50"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="55" t="s">
+      <c r="C34" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="46" t="str">
+      <c r="D34" s="47" t="str">
         <f aca="false">IF(E34&gt;0,CONCATENATE(ROUND((((E39/E34)-1)*100),2)," %"),"")</f>
         <v/>
       </c>
-      <c r="E34" s="56"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="58"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="59"/>
+      <c r="H34" s="59"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="53" t="s">
+      <c r="C35" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="46" t="str">
+      <c r="D35" s="47" t="str">
         <f aca="false">IF(E35&gt;0,CONCATENATE(ROUND((((E39/E35)-1)*100),2)," %"),"")</f>
         <v/>
       </c>
-      <c r="E35" s="54"/>
+      <c r="E35" s="55"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="53" t="s">
+      <c r="C36" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="46" t="str">
+      <c r="D36" s="47" t="str">
         <f aca="false">IF(E36&gt;0,CONCATENATE(ROUND((((E40/E36)-1)*100),2)," %"),"")</f>
         <v/>
       </c>
-      <c r="E36" s="54"/>
+      <c r="E36" s="55"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="53" t="s">
+      <c r="C37" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="D37" s="46" t="str">
+      <c r="D37" s="47" t="str">
         <f aca="false">IF(E37&gt;0,CONCATENATE(ROUND((((E39/E37)-1)*100),2)," %"),"")</f>
         <v/>
       </c>
-      <c r="E37" s="54"/>
+      <c r="E37" s="55"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="55" t="s">
+      <c r="C38" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="46" t="str">
+      <c r="D38" s="47" t="str">
         <f aca="false">IF(E38&gt;0,CONCATENATE(ROUND((((E42/E38)-1)*100),2)," %"),"")</f>
         <v/>
       </c>
-      <c r="E38" s="59"/>
+      <c r="E38" s="60"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="60" t="s">
+      <c r="C39" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="E39" s="61"/>
+      <c r="E39" s="62"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="45" t="s">
+      <c r="C40" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="D40" s="46" t="str">
+      <c r="D40" s="47" t="str">
         <f aca="false">IF(E40&gt;0,CONCATENATE(ROUND(((E39/E40)*100),2)," €/m2"),"")</f>
         <v/>
       </c>
-      <c r="E40" s="62"/>
+      <c r="E40" s="63"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="53" t="s">
+      <c r="C41" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="D41" s="46" t="str">
+      <c r="D41" s="47" t="str">
         <f aca="false">IF(E41&gt;0,CONCATENATE(ROUND(((E41/E39)*100),2)," %"),"")</f>
         <v/>
       </c>
-      <c r="E41" s="63"/>
+      <c r="E41" s="64"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="53" t="s">
+      <c r="C42" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="D42" s="46" t="str">
+      <c r="D42" s="47" t="str">
         <f aca="false">IF(E42&gt;0,CONCATENATE(ROUND(((E42/E39)*100),2)," %"),"")</f>
         <v/>
       </c>
-      <c r="E42" s="63"/>
+      <c r="E42" s="64"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="53" t="s">
+      <c r="C43" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="D43" s="46" t="str">
+      <c r="D43" s="47" t="str">
         <f aca="false">IF(E43&gt;0,CONCATENATE(ROUND(((E43/E39)*100),2)," %"),"")</f>
         <v/>
       </c>
-      <c r="E43" s="63"/>
+      <c r="E43" s="64"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="60" t="s">
+      <c r="C44" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="D44" s="46" t="str">
+      <c r="D44" s="47" t="str">
         <f aca="false">IF(E44&gt;0,CONCATENATE(ROUND((((E44/E39)-1)*100),2)," %"),"")</f>
         <v/>
       </c>
-      <c r="E44" s="64"/>
+      <c r="E44" s="65"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="46" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C46" s="65" t="s">
+      <c r="C46" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="D46" s="65"/>
-      <c r="E46" s="65"/>
-      <c r="F46" s="65"/>
-      <c r="G46" s="65"/>
-      <c r="H46" s="65"/>
-      <c r="I46" s="65"/>
-      <c r="J46" s="65"/>
-      <c r="K46" s="65"/>
-      <c r="L46" s="65"/>
+      <c r="D46" s="66"/>
+      <c r="E46" s="66"/>
+      <c r="F46" s="66"/>
+      <c r="G46" s="66"/>
+      <c r="H46" s="66"/>
+      <c r="I46" s="66"/>
+      <c r="J46" s="66"/>
+      <c r="K46" s="66"/>
+      <c r="L46" s="66"/>
       <c r="M46" s="5"/>
     </row>
     <row r="47" s="5" customFormat="true" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="48" s="66" customFormat="true" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E48" s="67" t="s">
+    <row r="48" s="67" customFormat="true" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E48" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="F48" s="67" t="s">
+      <c r="F48" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="G48" s="67" t="s">
+      <c r="G48" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="H48" s="67" t="s">
+      <c r="H48" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="I48" s="67" t="s">
+      <c r="I48" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="J48" s="67" t="s">
+      <c r="J48" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="K48" s="67" t="s">
+      <c r="K48" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="L48" s="67" t="s">
+      <c r="L48" s="68" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="49" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E49" s="68"/>
-      <c r="F49" s="68"/>
-      <c r="G49" s="68"/>
-      <c r="H49" s="69"/>
-      <c r="I49" s="70"/>
-      <c r="J49" s="71"/>
-      <c r="K49" s="71"/>
-      <c r="L49" s="71"/>
-    </row>
-    <row r="50" s="72" customFormat="true" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E49" s="69"/>
+      <c r="F49" s="69"/>
+      <c r="G49" s="69"/>
+      <c r="H49" s="70"/>
+      <c r="I49" s="71"/>
+      <c r="J49" s="72"/>
+      <c r="K49" s="72"/>
+      <c r="L49" s="72"/>
+    </row>
+    <row r="50" s="5" customFormat="true" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H50" s="73"/>
       <c r="I50" s="74"/>
       <c r="J50" s="75"/>
@@ -2630,13 +2612,13 @@
       <c r="C53" s="78"/>
       <c r="D53" s="78"/>
       <c r="E53" s="78"/>
-      <c r="F53" s="68"/>
-      <c r="G53" s="68"/>
-      <c r="H53" s="68"/>
-      <c r="I53" s="68"/>
-      <c r="J53" s="68"/>
-      <c r="K53" s="68"/>
-      <c r="L53" s="68"/>
+      <c r="F53" s="69"/>
+      <c r="G53" s="69"/>
+      <c r="H53" s="69"/>
+      <c r="I53" s="69"/>
+      <c r="J53" s="69"/>
+      <c r="K53" s="69"/>
+      <c r="L53" s="69"/>
     </row>
     <row r="54" s="5" customFormat="true" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="5" t="n">
@@ -2645,13 +2627,13 @@
       <c r="C54" s="78"/>
       <c r="D54" s="78"/>
       <c r="E54" s="78"/>
-      <c r="F54" s="68"/>
-      <c r="G54" s="68"/>
-      <c r="H54" s="68"/>
-      <c r="I54" s="68"/>
-      <c r="J54" s="68"/>
-      <c r="K54" s="68"/>
-      <c r="L54" s="68"/>
+      <c r="F54" s="69"/>
+      <c r="G54" s="69"/>
+      <c r="H54" s="69"/>
+      <c r="I54" s="69"/>
+      <c r="J54" s="69"/>
+      <c r="K54" s="69"/>
+      <c r="L54" s="69"/>
     </row>
     <row r="55" s="5" customFormat="true" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="5" t="n">
@@ -2660,13 +2642,13 @@
       <c r="C55" s="78"/>
       <c r="D55" s="78"/>
       <c r="E55" s="78"/>
-      <c r="F55" s="68"/>
-      <c r="G55" s="68"/>
-      <c r="H55" s="68"/>
-      <c r="I55" s="68"/>
-      <c r="J55" s="68"/>
-      <c r="K55" s="68"/>
-      <c r="L55" s="68"/>
+      <c r="F55" s="69"/>
+      <c r="G55" s="69"/>
+      <c r="H55" s="69"/>
+      <c r="I55" s="69"/>
+      <c r="J55" s="69"/>
+      <c r="K55" s="69"/>
+      <c r="L55" s="69"/>
     </row>
     <row r="56" s="5" customFormat="true" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="57" s="5" customFormat="true" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2674,18 +2656,18 @@
       <c r="B58" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C58" s="65" t="s">
+      <c r="C58" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="D58" s="65"/>
-      <c r="E58" s="65"/>
-      <c r="F58" s="65"/>
-      <c r="G58" s="65"/>
-      <c r="H58" s="65"/>
-      <c r="I58" s="65"/>
-      <c r="J58" s="65"/>
-      <c r="K58" s="65"/>
-      <c r="L58" s="65"/>
+      <c r="D58" s="66"/>
+      <c r="E58" s="66"/>
+      <c r="F58" s="66"/>
+      <c r="G58" s="66"/>
+      <c r="H58" s="66"/>
+      <c r="I58" s="66"/>
+      <c r="J58" s="66"/>
+      <c r="K58" s="66"/>
+      <c r="L58" s="66"/>
       <c r="M58" s="5"/>
     </row>
     <row r="59" s="5" customFormat="true" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2785,18 +2767,18 @@
       <c r="B68" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C68" s="65" t="s">
+      <c r="C68" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="D68" s="65"/>
-      <c r="E68" s="65"/>
-      <c r="F68" s="65"/>
-      <c r="G68" s="65"/>
-      <c r="H68" s="65"/>
-      <c r="I68" s="65"/>
-      <c r="J68" s="65"/>
-      <c r="K68" s="65"/>
-      <c r="L68" s="65"/>
+      <c r="D68" s="66"/>
+      <c r="E68" s="66"/>
+      <c r="F68" s="66"/>
+      <c r="G68" s="66"/>
+      <c r="H68" s="66"/>
+      <c r="I68" s="66"/>
+      <c r="J68" s="66"/>
+      <c r="K68" s="66"/>
+      <c r="L68" s="66"/>
       <c r="M68" s="5"/>
     </row>
     <row r="69" s="5" customFormat="true" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2937,18 +2919,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B4:AH21"/>
+  <dimension ref="B4:AH22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topRight" activeCell="AD19" activeCellId="0" sqref="AD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.57"/>
@@ -2957,9 +2939,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="28.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="89" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="89" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="25.85"/>
@@ -3136,577 +3118,494 @@
     <row r="8" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="100"/>
       <c r="C8" s="101"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="101"/>
       <c r="F8" s="101"/>
-      <c r="G8" s="103"/>
-      <c r="H8" s="104"/>
-      <c r="I8" s="104"/>
-      <c r="J8" s="103"/>
-      <c r="K8" s="104"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="104"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="102"/>
+      <c r="I8" s="102"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="102"/>
+      <c r="L8" s="103"/>
+      <c r="M8" s="102"/>
       <c r="N8" s="101"/>
-      <c r="O8" s="104"/>
+      <c r="O8" s="102"/>
       <c r="P8" s="101"/>
-      <c r="Q8" s="104"/>
-      <c r="R8" s="104"/>
-      <c r="S8" s="104"/>
-      <c r="T8" s="106"/>
-      <c r="U8" s="106"/>
-      <c r="V8" s="107"/>
-      <c r="W8" s="106"/>
-      <c r="X8" s="108"/>
-      <c r="Y8" s="106"/>
-      <c r="Z8" s="106"/>
-      <c r="AA8" s="106"/>
-      <c r="AB8" s="109" t="e">
-        <f aca="false">ROUND((AA8/L8),2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC8" s="110"/>
-      <c r="AD8" s="111"/>
-      <c r="AE8" s="111"/>
-      <c r="AF8" s="112" t="n">
-        <f aca="false">AA8 - AC8</f>
-        <v>0</v>
-      </c>
-      <c r="AG8" s="113"/>
-      <c r="AH8" s="103"/>
+      <c r="Q8" s="102"/>
+      <c r="R8" s="102"/>
+      <c r="S8" s="102"/>
+      <c r="T8" s="104"/>
+      <c r="U8" s="104"/>
+      <c r="V8" s="105"/>
+      <c r="W8" s="104"/>
+      <c r="X8" s="105"/>
+      <c r="Y8" s="104"/>
+      <c r="Z8" s="104"/>
+      <c r="AA8" s="104"/>
+      <c r="AB8" s="103"/>
+      <c r="AC8" s="106"/>
+      <c r="AD8" s="105"/>
+      <c r="AE8" s="105"/>
+      <c r="AF8" s="105"/>
+      <c r="AG8" s="107"/>
+      <c r="AH8" s="100"/>
     </row>
     <row r="9" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="100"/>
       <c r="C9" s="101"/>
-      <c r="D9" s="102"/>
-      <c r="E9" s="102"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="101"/>
       <c r="F9" s="101"/>
-      <c r="G9" s="103"/>
-      <c r="H9" s="104"/>
-      <c r="I9" s="104"/>
-      <c r="J9" s="103"/>
-      <c r="K9" s="104"/>
-      <c r="L9" s="105"/>
-      <c r="M9" s="104"/>
+      <c r="G9" s="100"/>
+      <c r="H9" s="102"/>
+      <c r="I9" s="102"/>
+      <c r="J9" s="100"/>
+      <c r="K9" s="102"/>
+      <c r="L9" s="103"/>
+      <c r="M9" s="102"/>
       <c r="N9" s="101"/>
-      <c r="O9" s="104"/>
+      <c r="O9" s="102"/>
       <c r="P9" s="101"/>
-      <c r="Q9" s="104"/>
-      <c r="R9" s="104"/>
-      <c r="S9" s="104"/>
-      <c r="T9" s="106"/>
-      <c r="U9" s="106"/>
-      <c r="V9" s="107"/>
-      <c r="W9" s="106"/>
-      <c r="X9" s="108"/>
-      <c r="Y9" s="106"/>
-      <c r="Z9" s="106"/>
-      <c r="AA9" s="106"/>
-      <c r="AB9" s="109" t="e">
-        <f aca="false">ROUND((AA9/L9),2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC9" s="110"/>
-      <c r="AD9" s="111"/>
-      <c r="AE9" s="111"/>
-      <c r="AF9" s="112" t="n">
-        <f aca="false">AA9 - AC9</f>
-        <v>0</v>
-      </c>
-      <c r="AG9" s="114"/>
-      <c r="AH9" s="103"/>
+      <c r="Q9" s="102"/>
+      <c r="R9" s="102"/>
+      <c r="S9" s="102"/>
+      <c r="T9" s="104"/>
+      <c r="U9" s="104"/>
+      <c r="V9" s="105"/>
+      <c r="W9" s="104"/>
+      <c r="X9" s="105"/>
+      <c r="Y9" s="104"/>
+      <c r="Z9" s="104"/>
+      <c r="AA9" s="104"/>
+      <c r="AB9" s="103"/>
+      <c r="AC9" s="106"/>
+      <c r="AD9" s="105"/>
+      <c r="AE9" s="105"/>
+      <c r="AF9" s="105"/>
+      <c r="AG9" s="107"/>
+      <c r="AH9" s="100"/>
     </row>
     <row r="10" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="100"/>
       <c r="C10" s="101"/>
-      <c r="D10" s="102"/>
-      <c r="E10" s="102"/>
+      <c r="D10" s="101"/>
+      <c r="E10" s="101"/>
       <c r="F10" s="101"/>
-      <c r="G10" s="103"/>
-      <c r="H10" s="104"/>
-      <c r="I10" s="104"/>
-      <c r="J10" s="103"/>
-      <c r="K10" s="104"/>
-      <c r="L10" s="105"/>
-      <c r="M10" s="104"/>
+      <c r="G10" s="100"/>
+      <c r="H10" s="102"/>
+      <c r="I10" s="102"/>
+      <c r="J10" s="100"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="103"/>
+      <c r="M10" s="102"/>
       <c r="N10" s="101"/>
-      <c r="O10" s="104"/>
+      <c r="O10" s="102"/>
       <c r="P10" s="101"/>
-      <c r="Q10" s="104"/>
-      <c r="R10" s="104"/>
-      <c r="S10" s="104"/>
-      <c r="T10" s="106"/>
-      <c r="U10" s="106"/>
-      <c r="V10" s="107"/>
-      <c r="W10" s="106"/>
-      <c r="X10" s="108"/>
-      <c r="Y10" s="106"/>
-      <c r="Z10" s="106"/>
-      <c r="AA10" s="106"/>
-      <c r="AB10" s="109" t="e">
-        <f aca="false">ROUND((AA10/L10),2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC10" s="110"/>
-      <c r="AD10" s="111"/>
-      <c r="AE10" s="111"/>
-      <c r="AF10" s="112" t="n">
-        <f aca="false">AA10 - AC10</f>
-        <v>0</v>
-      </c>
-      <c r="AG10" s="114"/>
-      <c r="AH10" s="103"/>
+      <c r="Q10" s="102"/>
+      <c r="R10" s="102"/>
+      <c r="S10" s="102"/>
+      <c r="T10" s="104"/>
+      <c r="U10" s="104"/>
+      <c r="V10" s="105"/>
+      <c r="W10" s="104"/>
+      <c r="X10" s="105"/>
+      <c r="Y10" s="104"/>
+      <c r="Z10" s="104"/>
+      <c r="AA10" s="104"/>
+      <c r="AB10" s="103"/>
+      <c r="AC10" s="106"/>
+      <c r="AD10" s="105"/>
+      <c r="AE10" s="105"/>
+      <c r="AF10" s="105"/>
+      <c r="AG10" s="107"/>
+      <c r="AH10" s="100"/>
     </row>
     <row r="11" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="100"/>
       <c r="C11" s="101"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="102"/>
+      <c r="D11" s="101"/>
+      <c r="E11" s="101"/>
       <c r="F11" s="101"/>
-      <c r="G11" s="103"/>
-      <c r="H11" s="104"/>
-      <c r="I11" s="104"/>
-      <c r="J11" s="103"/>
-      <c r="K11" s="104"/>
-      <c r="L11" s="105"/>
-      <c r="M11" s="104"/>
+      <c r="G11" s="100"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="102"/>
+      <c r="J11" s="100"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="103"/>
+      <c r="M11" s="102"/>
       <c r="N11" s="101"/>
-      <c r="O11" s="104"/>
+      <c r="O11" s="102"/>
       <c r="P11" s="101"/>
-      <c r="Q11" s="104"/>
-      <c r="R11" s="104"/>
-      <c r="S11" s="104"/>
-      <c r="T11" s="106"/>
-      <c r="U11" s="106"/>
-      <c r="V11" s="107"/>
-      <c r="W11" s="106"/>
-      <c r="X11" s="108"/>
-      <c r="Y11" s="106"/>
-      <c r="Z11" s="106"/>
-      <c r="AA11" s="106"/>
-      <c r="AB11" s="109" t="e">
-        <f aca="false">ROUND((AA11/L11),2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC11" s="110"/>
-      <c r="AD11" s="111"/>
-      <c r="AE11" s="111"/>
-      <c r="AF11" s="112" t="n">
-        <f aca="false">AA11 - AC11</f>
-        <v>0</v>
-      </c>
-      <c r="AG11" s="114"/>
-      <c r="AH11" s="103"/>
+      <c r="Q11" s="102"/>
+      <c r="R11" s="102"/>
+      <c r="S11" s="102"/>
+      <c r="T11" s="104"/>
+      <c r="U11" s="104"/>
+      <c r="V11" s="105"/>
+      <c r="W11" s="104"/>
+      <c r="X11" s="105"/>
+      <c r="Y11" s="104"/>
+      <c r="Z11" s="104"/>
+      <c r="AA11" s="104"/>
+      <c r="AB11" s="103"/>
+      <c r="AC11" s="106"/>
+      <c r="AD11" s="105"/>
+      <c r="AE11" s="105"/>
+      <c r="AF11" s="105"/>
+      <c r="AG11" s="107"/>
+      <c r="AH11" s="100"/>
     </row>
     <row r="12" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="100"/>
       <c r="C12" s="101"/>
-      <c r="D12" s="102"/>
-      <c r="E12" s="102"/>
+      <c r="D12" s="101"/>
+      <c r="E12" s="101"/>
       <c r="F12" s="101"/>
-      <c r="G12" s="103"/>
-      <c r="H12" s="104"/>
-      <c r="I12" s="104"/>
-      <c r="J12" s="103"/>
-      <c r="K12" s="104"/>
-      <c r="L12" s="105"/>
-      <c r="M12" s="104"/>
+      <c r="G12" s="100"/>
+      <c r="H12" s="102"/>
+      <c r="I12" s="102"/>
+      <c r="J12" s="100"/>
+      <c r="K12" s="102"/>
+      <c r="L12" s="103"/>
+      <c r="M12" s="102"/>
       <c r="N12" s="101"/>
-      <c r="O12" s="104"/>
+      <c r="O12" s="102"/>
       <c r="P12" s="101"/>
-      <c r="Q12" s="104"/>
-      <c r="R12" s="104"/>
-      <c r="S12" s="104"/>
-      <c r="T12" s="106"/>
-      <c r="U12" s="106"/>
-      <c r="V12" s="115"/>
-      <c r="W12" s="106"/>
-      <c r="X12" s="116"/>
-      <c r="Y12" s="106"/>
-      <c r="Z12" s="106"/>
-      <c r="AA12" s="106"/>
-      <c r="AB12" s="109" t="e">
-        <f aca="false">ROUND((AA12/L12),2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC12" s="110"/>
-      <c r="AD12" s="111"/>
-      <c r="AE12" s="111"/>
-      <c r="AF12" s="112" t="n">
-        <f aca="false">AA12 - AC12</f>
-        <v>0</v>
-      </c>
-      <c r="AG12" s="114"/>
-      <c r="AH12" s="103"/>
+      <c r="Q12" s="102"/>
+      <c r="R12" s="102"/>
+      <c r="S12" s="102"/>
+      <c r="T12" s="104"/>
+      <c r="U12" s="104"/>
+      <c r="V12" s="105"/>
+      <c r="W12" s="104"/>
+      <c r="X12" s="105"/>
+      <c r="Y12" s="104"/>
+      <c r="Z12" s="104"/>
+      <c r="AA12" s="104"/>
+      <c r="AB12" s="103"/>
+      <c r="AC12" s="106"/>
+      <c r="AD12" s="105"/>
+      <c r="AE12" s="105"/>
+      <c r="AF12" s="105"/>
+      <c r="AG12" s="107"/>
+      <c r="AH12" s="100"/>
     </row>
     <row r="13" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="100"/>
       <c r="C13" s="101"/>
-      <c r="D13" s="102"/>
-      <c r="E13" s="102"/>
+      <c r="D13" s="101"/>
+      <c r="E13" s="101"/>
       <c r="F13" s="101"/>
-      <c r="G13" s="103"/>
-      <c r="H13" s="104"/>
-      <c r="I13" s="104"/>
-      <c r="J13" s="103"/>
-      <c r="K13" s="104"/>
-      <c r="L13" s="105"/>
-      <c r="M13" s="104"/>
+      <c r="G13" s="100"/>
+      <c r="H13" s="102"/>
+      <c r="I13" s="102"/>
+      <c r="J13" s="100"/>
+      <c r="K13" s="102"/>
+      <c r="L13" s="103"/>
+      <c r="M13" s="102"/>
       <c r="N13" s="101"/>
-      <c r="O13" s="104"/>
+      <c r="O13" s="102"/>
       <c r="P13" s="101"/>
-      <c r="Q13" s="104"/>
-      <c r="R13" s="104"/>
-      <c r="S13" s="104"/>
-      <c r="T13" s="106"/>
-      <c r="U13" s="106"/>
-      <c r="V13" s="107"/>
-      <c r="W13" s="106"/>
-      <c r="X13" s="108"/>
-      <c r="Y13" s="106"/>
-      <c r="Z13" s="106"/>
-      <c r="AA13" s="106"/>
-      <c r="AB13" s="109" t="e">
-        <f aca="false">ROUND((AA13/L13),2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC13" s="110"/>
-      <c r="AD13" s="111"/>
-      <c r="AE13" s="111"/>
-      <c r="AF13" s="112" t="n">
-        <f aca="false">AA13 - AC13</f>
-        <v>0</v>
-      </c>
-      <c r="AG13" s="114"/>
-      <c r="AH13" s="103"/>
+      <c r="Q13" s="102"/>
+      <c r="R13" s="102"/>
+      <c r="S13" s="102"/>
+      <c r="T13" s="104"/>
+      <c r="U13" s="104"/>
+      <c r="V13" s="105"/>
+      <c r="W13" s="104"/>
+      <c r="X13" s="105"/>
+      <c r="Y13" s="104"/>
+      <c r="Z13" s="104"/>
+      <c r="AA13" s="104"/>
+      <c r="AB13" s="103"/>
+      <c r="AC13" s="106"/>
+      <c r="AD13" s="105"/>
+      <c r="AE13" s="105"/>
+      <c r="AF13" s="105"/>
+      <c r="AG13" s="107"/>
+      <c r="AH13" s="100"/>
     </row>
     <row r="14" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="100"/>
       <c r="C14" s="101"/>
-      <c r="D14" s="102"/>
-      <c r="E14" s="102"/>
+      <c r="D14" s="101"/>
+      <c r="E14" s="101"/>
       <c r="F14" s="101"/>
-      <c r="G14" s="103"/>
-      <c r="H14" s="104"/>
-      <c r="I14" s="104"/>
-      <c r="J14" s="103"/>
-      <c r="K14" s="104"/>
-      <c r="L14" s="105"/>
-      <c r="M14" s="104"/>
+      <c r="G14" s="100"/>
+      <c r="H14" s="102"/>
+      <c r="I14" s="102"/>
+      <c r="J14" s="100"/>
+      <c r="K14" s="102"/>
+      <c r="L14" s="103"/>
+      <c r="M14" s="102"/>
       <c r="N14" s="101"/>
-      <c r="O14" s="104"/>
+      <c r="O14" s="102"/>
       <c r="P14" s="101"/>
-      <c r="Q14" s="104"/>
-      <c r="R14" s="104"/>
-      <c r="S14" s="104"/>
-      <c r="T14" s="106"/>
-      <c r="U14" s="106"/>
-      <c r="V14" s="107"/>
-      <c r="W14" s="106"/>
-      <c r="X14" s="108"/>
-      <c r="Y14" s="106"/>
-      <c r="Z14" s="106"/>
-      <c r="AA14" s="106"/>
-      <c r="AB14" s="109" t="e">
-        <f aca="false">ROUND((AA14/L14),2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC14" s="110"/>
-      <c r="AD14" s="111"/>
-      <c r="AE14" s="111"/>
-      <c r="AF14" s="112" t="n">
-        <f aca="false">AA14 - AC14</f>
-        <v>0</v>
-      </c>
-      <c r="AG14" s="114"/>
-      <c r="AH14" s="103"/>
+      <c r="Q14" s="102"/>
+      <c r="R14" s="102"/>
+      <c r="S14" s="102"/>
+      <c r="T14" s="104"/>
+      <c r="U14" s="104"/>
+      <c r="V14" s="105"/>
+      <c r="W14" s="104"/>
+      <c r="X14" s="105"/>
+      <c r="Y14" s="104"/>
+      <c r="Z14" s="104"/>
+      <c r="AA14" s="104"/>
+      <c r="AB14" s="103"/>
+      <c r="AC14" s="106"/>
+      <c r="AD14" s="105"/>
+      <c r="AE14" s="105"/>
+      <c r="AF14" s="105"/>
+      <c r="AG14" s="107"/>
+      <c r="AH14" s="100"/>
     </row>
     <row r="15" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="100"/>
       <c r="C15" s="101"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="102"/>
+      <c r="D15" s="101"/>
+      <c r="E15" s="101"/>
       <c r="F15" s="101"/>
-      <c r="G15" s="103"/>
-      <c r="H15" s="104"/>
-      <c r="I15" s="104"/>
-      <c r="J15" s="103"/>
-      <c r="K15" s="104"/>
-      <c r="L15" s="105"/>
-      <c r="M15" s="104"/>
+      <c r="G15" s="100"/>
+      <c r="H15" s="102"/>
+      <c r="I15" s="102"/>
+      <c r="J15" s="100"/>
+      <c r="K15" s="102"/>
+      <c r="L15" s="103"/>
+      <c r="M15" s="102"/>
       <c r="N15" s="101"/>
-      <c r="O15" s="104"/>
+      <c r="O15" s="102"/>
       <c r="P15" s="101"/>
-      <c r="Q15" s="104"/>
-      <c r="R15" s="104"/>
-      <c r="S15" s="104"/>
-      <c r="T15" s="106"/>
-      <c r="U15" s="106"/>
-      <c r="V15" s="115"/>
-      <c r="W15" s="106"/>
-      <c r="X15" s="116"/>
-      <c r="Y15" s="106"/>
-      <c r="Z15" s="106"/>
-      <c r="AA15" s="106"/>
-      <c r="AB15" s="109" t="e">
-        <f aca="false">ROUND((AA15/L15),2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC15" s="110"/>
-      <c r="AD15" s="111"/>
-      <c r="AE15" s="111"/>
-      <c r="AF15" s="112" t="n">
-        <f aca="false">AA15 - AC15</f>
-        <v>0</v>
-      </c>
-      <c r="AG15" s="114"/>
-      <c r="AH15" s="103"/>
+      <c r="Q15" s="102"/>
+      <c r="R15" s="102"/>
+      <c r="S15" s="102"/>
+      <c r="T15" s="104"/>
+      <c r="U15" s="104"/>
+      <c r="V15" s="105"/>
+      <c r="W15" s="104"/>
+      <c r="X15" s="105"/>
+      <c r="Y15" s="104"/>
+      <c r="Z15" s="104"/>
+      <c r="AA15" s="104"/>
+      <c r="AB15" s="103"/>
+      <c r="AC15" s="106"/>
+      <c r="AD15" s="105"/>
+      <c r="AE15" s="105"/>
+      <c r="AF15" s="105"/>
+      <c r="AG15" s="107"/>
+      <c r="AH15" s="100"/>
     </row>
     <row r="16" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="100"/>
       <c r="C16" s="101"/>
-      <c r="D16" s="102"/>
-      <c r="E16" s="102"/>
+      <c r="D16" s="101"/>
+      <c r="E16" s="101"/>
       <c r="F16" s="101"/>
-      <c r="G16" s="103"/>
-      <c r="H16" s="104"/>
-      <c r="I16" s="104"/>
-      <c r="J16" s="103"/>
-      <c r="K16" s="104"/>
-      <c r="L16" s="105"/>
-      <c r="M16" s="104"/>
+      <c r="G16" s="100"/>
+      <c r="H16" s="102"/>
+      <c r="I16" s="102"/>
+      <c r="J16" s="100"/>
+      <c r="K16" s="102"/>
+      <c r="L16" s="103"/>
+      <c r="M16" s="102"/>
       <c r="N16" s="101"/>
-      <c r="O16" s="104"/>
+      <c r="O16" s="102"/>
       <c r="P16" s="101"/>
-      <c r="Q16" s="104"/>
-      <c r="R16" s="104"/>
-      <c r="S16" s="104"/>
-      <c r="T16" s="106"/>
-      <c r="U16" s="106"/>
-      <c r="V16" s="107"/>
-      <c r="W16" s="106"/>
-      <c r="X16" s="108"/>
-      <c r="Y16" s="106"/>
-      <c r="Z16" s="106"/>
-      <c r="AA16" s="106"/>
-      <c r="AB16" s="109" t="e">
-        <f aca="false">ROUND((AA16/L16),2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC16" s="110"/>
-      <c r="AD16" s="111"/>
-      <c r="AE16" s="111"/>
-      <c r="AF16" s="112" t="n">
-        <f aca="false">AA16 - AC16</f>
-        <v>0</v>
-      </c>
-      <c r="AG16" s="114"/>
-      <c r="AH16" s="103"/>
+      <c r="Q16" s="102"/>
+      <c r="R16" s="102"/>
+      <c r="S16" s="102"/>
+      <c r="T16" s="104"/>
+      <c r="U16" s="104"/>
+      <c r="V16" s="105"/>
+      <c r="W16" s="104"/>
+      <c r="X16" s="105"/>
+      <c r="Y16" s="104"/>
+      <c r="Z16" s="104"/>
+      <c r="AA16" s="104"/>
+      <c r="AB16" s="103"/>
+      <c r="AC16" s="106"/>
+      <c r="AD16" s="105"/>
+      <c r="AE16" s="105"/>
+      <c r="AF16" s="105"/>
+      <c r="AG16" s="107"/>
+      <c r="AH16" s="100"/>
     </row>
     <row r="17" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="100"/>
       <c r="C17" s="101"/>
-      <c r="D17" s="102"/>
-      <c r="E17" s="102"/>
+      <c r="D17" s="101"/>
+      <c r="E17" s="101"/>
       <c r="F17" s="101"/>
-      <c r="G17" s="103"/>
-      <c r="H17" s="104"/>
-      <c r="I17" s="104"/>
-      <c r="J17" s="103"/>
-      <c r="K17" s="104"/>
-      <c r="L17" s="105"/>
-      <c r="M17" s="104"/>
+      <c r="G17" s="100"/>
+      <c r="H17" s="102"/>
+      <c r="I17" s="102"/>
+      <c r="J17" s="100"/>
+      <c r="K17" s="102"/>
+      <c r="L17" s="103"/>
+      <c r="M17" s="102"/>
       <c r="N17" s="101"/>
-      <c r="O17" s="104"/>
+      <c r="O17" s="102"/>
       <c r="P17" s="101"/>
-      <c r="Q17" s="104"/>
-      <c r="R17" s="104"/>
-      <c r="S17" s="104"/>
-      <c r="T17" s="106"/>
-      <c r="U17" s="106"/>
-      <c r="V17" s="107"/>
-      <c r="W17" s="106"/>
-      <c r="X17" s="108"/>
-      <c r="Y17" s="106"/>
-      <c r="Z17" s="106"/>
-      <c r="AA17" s="106"/>
-      <c r="AB17" s="109" t="e">
-        <f aca="false">ROUND((AA17/L17),2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC17" s="110"/>
-      <c r="AD17" s="111"/>
-      <c r="AE17" s="111"/>
-      <c r="AF17" s="112" t="n">
-        <f aca="false">AA17 - AC17</f>
-        <v>0</v>
-      </c>
-      <c r="AG17" s="114"/>
-      <c r="AH17" s="103"/>
+      <c r="Q17" s="102"/>
+      <c r="R17" s="102"/>
+      <c r="S17" s="102"/>
+      <c r="T17" s="104"/>
+      <c r="U17" s="104"/>
+      <c r="V17" s="105"/>
+      <c r="W17" s="104"/>
+      <c r="X17" s="105"/>
+      <c r="Y17" s="104"/>
+      <c r="Z17" s="104"/>
+      <c r="AA17" s="104"/>
+      <c r="AB17" s="103"/>
+      <c r="AC17" s="106"/>
+      <c r="AD17" s="105"/>
+      <c r="AE17" s="105"/>
+      <c r="AF17" s="105"/>
+      <c r="AG17" s="107"/>
+      <c r="AH17" s="100"/>
     </row>
     <row r="18" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="100"/>
       <c r="C18" s="101"/>
-      <c r="D18" s="102"/>
-      <c r="E18" s="102"/>
+      <c r="D18" s="101"/>
+      <c r="E18" s="101"/>
       <c r="F18" s="101"/>
-      <c r="G18" s="103"/>
-      <c r="H18" s="104"/>
-      <c r="I18" s="104"/>
-      <c r="J18" s="103"/>
-      <c r="K18" s="104"/>
-      <c r="L18" s="105"/>
-      <c r="M18" s="104"/>
+      <c r="G18" s="100"/>
+      <c r="H18" s="102"/>
+      <c r="I18" s="102"/>
+      <c r="J18" s="100"/>
+      <c r="K18" s="102"/>
+      <c r="L18" s="103"/>
+      <c r="M18" s="102"/>
       <c r="N18" s="101"/>
-      <c r="O18" s="104"/>
+      <c r="O18" s="102"/>
       <c r="P18" s="101"/>
-      <c r="Q18" s="104"/>
-      <c r="R18" s="104"/>
-      <c r="S18" s="104"/>
-      <c r="T18" s="106"/>
-      <c r="U18" s="106"/>
-      <c r="V18" s="107"/>
-      <c r="W18" s="106"/>
-      <c r="X18" s="108"/>
-      <c r="Y18" s="106"/>
-      <c r="Z18" s="106"/>
-      <c r="AA18" s="106"/>
-      <c r="AB18" s="109" t="e">
-        <f aca="false">ROUND((AA18/L18),2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC18" s="110"/>
-      <c r="AD18" s="111"/>
-      <c r="AE18" s="111"/>
-      <c r="AF18" s="112" t="n">
-        <f aca="false">AA18 - AC18</f>
-        <v>0</v>
-      </c>
-      <c r="AG18" s="114"/>
-      <c r="AH18" s="103"/>
+      <c r="Q18" s="102"/>
+      <c r="R18" s="102"/>
+      <c r="S18" s="102"/>
+      <c r="T18" s="104"/>
+      <c r="U18" s="104"/>
+      <c r="V18" s="105"/>
+      <c r="W18" s="104"/>
+      <c r="X18" s="105"/>
+      <c r="Y18" s="104"/>
+      <c r="Z18" s="104"/>
+      <c r="AA18" s="104"/>
+      <c r="AB18" s="103"/>
+      <c r="AC18" s="106"/>
+      <c r="AD18" s="105"/>
+      <c r="AE18" s="105"/>
+      <c r="AF18" s="105"/>
+      <c r="AG18" s="107"/>
+      <c r="AH18" s="100"/>
     </row>
     <row r="19" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="100"/>
       <c r="C19" s="101"/>
-      <c r="D19" s="102"/>
-      <c r="E19" s="102"/>
+      <c r="D19" s="101"/>
+      <c r="E19" s="101"/>
       <c r="F19" s="101"/>
-      <c r="G19" s="103"/>
-      <c r="H19" s="104"/>
-      <c r="I19" s="104"/>
-      <c r="J19" s="103"/>
-      <c r="K19" s="104"/>
-      <c r="L19" s="105"/>
-      <c r="M19" s="104"/>
+      <c r="G19" s="100"/>
+      <c r="H19" s="102"/>
+      <c r="I19" s="102"/>
+      <c r="J19" s="100"/>
+      <c r="K19" s="102"/>
+      <c r="L19" s="103"/>
+      <c r="M19" s="102"/>
       <c r="N19" s="101"/>
-      <c r="O19" s="104"/>
+      <c r="O19" s="102"/>
       <c r="P19" s="101"/>
-      <c r="Q19" s="104"/>
-      <c r="R19" s="104"/>
-      <c r="S19" s="104"/>
-      <c r="T19" s="106"/>
-      <c r="U19" s="106"/>
-      <c r="V19" s="107"/>
-      <c r="W19" s="106"/>
-      <c r="X19" s="108"/>
-      <c r="Y19" s="106"/>
-      <c r="Z19" s="106"/>
-      <c r="AA19" s="106"/>
-      <c r="AB19" s="109" t="e">
-        <f aca="false">ROUND((AA19/L19),2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC19" s="110"/>
-      <c r="AD19" s="111"/>
-      <c r="AE19" s="111"/>
-      <c r="AF19" s="112" t="n">
-        <f aca="false">AA19 - AC19</f>
-        <v>0</v>
-      </c>
-      <c r="AG19" s="114"/>
-      <c r="AH19" s="103"/>
+      <c r="Q19" s="102"/>
+      <c r="R19" s="102"/>
+      <c r="S19" s="102"/>
+      <c r="T19" s="104"/>
+      <c r="U19" s="104"/>
+      <c r="V19" s="105"/>
+      <c r="W19" s="104"/>
+      <c r="X19" s="105"/>
+      <c r="Y19" s="104"/>
+      <c r="Z19" s="104"/>
+      <c r="AA19" s="104"/>
+      <c r="AB19" s="103"/>
+      <c r="AC19" s="106"/>
+      <c r="AD19" s="105"/>
+      <c r="AE19" s="105"/>
+      <c r="AF19" s="105"/>
+      <c r="AG19" s="107"/>
+      <c r="AH19" s="100"/>
     </row>
     <row r="20" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="100"/>
       <c r="C20" s="101"/>
-      <c r="D20" s="102"/>
-      <c r="E20" s="102"/>
+      <c r="D20" s="101"/>
+      <c r="E20" s="101"/>
       <c r="F20" s="101"/>
-      <c r="G20" s="103"/>
-      <c r="H20" s="104"/>
-      <c r="I20" s="104"/>
-      <c r="J20" s="103"/>
-      <c r="K20" s="104"/>
-      <c r="L20" s="105"/>
-      <c r="M20" s="104"/>
+      <c r="G20" s="100"/>
+      <c r="H20" s="102"/>
+      <c r="I20" s="102"/>
+      <c r="J20" s="100"/>
+      <c r="K20" s="102"/>
+      <c r="L20" s="103"/>
+      <c r="M20" s="102"/>
       <c r="N20" s="101"/>
-      <c r="O20" s="104"/>
+      <c r="O20" s="102"/>
       <c r="P20" s="101"/>
-      <c r="Q20" s="104"/>
-      <c r="R20" s="104"/>
-      <c r="S20" s="104"/>
-      <c r="T20" s="106"/>
-      <c r="U20" s="106"/>
-      <c r="V20" s="107"/>
-      <c r="W20" s="106"/>
-      <c r="X20" s="108"/>
-      <c r="Y20" s="106"/>
-      <c r="Z20" s="106"/>
-      <c r="AA20" s="106"/>
-      <c r="AB20" s="109" t="e">
-        <f aca="false">ROUND((AA20/L20),2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC20" s="110"/>
-      <c r="AD20" s="111"/>
-      <c r="AE20" s="111"/>
-      <c r="AF20" s="112" t="n">
-        <f aca="false">AA20 - AC20</f>
-        <v>0</v>
-      </c>
-      <c r="AG20" s="114"/>
-      <c r="AH20" s="103"/>
+      <c r="Q20" s="102"/>
+      <c r="R20" s="102"/>
+      <c r="S20" s="102"/>
+      <c r="T20" s="104"/>
+      <c r="U20" s="104"/>
+      <c r="V20" s="105"/>
+      <c r="W20" s="104"/>
+      <c r="X20" s="105"/>
+      <c r="Y20" s="104"/>
+      <c r="Z20" s="104"/>
+      <c r="AA20" s="104"/>
+      <c r="AB20" s="103"/>
+      <c r="AC20" s="106"/>
+      <c r="AD20" s="105"/>
+      <c r="AE20" s="105"/>
+      <c r="AF20" s="105"/>
+      <c r="AG20" s="107"/>
+      <c r="AH20" s="100"/>
     </row>
     <row r="21" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="100"/>
       <c r="C21" s="101"/>
-      <c r="D21" s="102"/>
-      <c r="E21" s="102"/>
+      <c r="D21" s="101"/>
+      <c r="E21" s="101"/>
       <c r="F21" s="101"/>
-      <c r="G21" s="103"/>
-      <c r="H21" s="104"/>
-      <c r="I21" s="104"/>
-      <c r="J21" s="103"/>
-      <c r="K21" s="104"/>
-      <c r="L21" s="105"/>
-      <c r="M21" s="104"/>
+      <c r="G21" s="100"/>
+      <c r="H21" s="102"/>
+      <c r="I21" s="102"/>
+      <c r="J21" s="100"/>
+      <c r="K21" s="102"/>
+      <c r="L21" s="103"/>
+      <c r="M21" s="102"/>
       <c r="N21" s="101"/>
-      <c r="O21" s="104"/>
+      <c r="O21" s="102"/>
       <c r="P21" s="101"/>
-      <c r="Q21" s="104"/>
-      <c r="R21" s="104"/>
-      <c r="S21" s="104"/>
-      <c r="T21" s="106"/>
-      <c r="U21" s="106"/>
-      <c r="V21" s="107"/>
-      <c r="W21" s="106"/>
-      <c r="X21" s="108"/>
-      <c r="Y21" s="106"/>
-      <c r="Z21" s="106"/>
-      <c r="AA21" s="106"/>
-      <c r="AB21" s="109" t="e">
-        <f aca="false">ROUND((AA21/L21),2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC21" s="110"/>
-      <c r="AD21" s="111"/>
-      <c r="AE21" s="111"/>
-      <c r="AF21" s="112" t="n">
-        <f aca="false">AA21 - AC21</f>
-        <v>0</v>
-      </c>
-      <c r="AG21" s="114"/>
-      <c r="AH21" s="103"/>
-    </row>
+      <c r="Q21" s="102"/>
+      <c r="R21" s="102"/>
+      <c r="S21" s="102"/>
+      <c r="T21" s="104"/>
+      <c r="U21" s="104"/>
+      <c r="V21" s="105"/>
+      <c r="W21" s="104"/>
+      <c r="X21" s="105"/>
+      <c r="Y21" s="104"/>
+      <c r="Z21" s="104"/>
+      <c r="AA21" s="104"/>
+      <c r="AB21" s="103"/>
+      <c r="AC21" s="106"/>
+      <c r="AD21" s="105"/>
+      <c r="AE21" s="105"/>
+      <c r="AF21" s="105"/>
+      <c r="AG21" s="107"/>
+      <c r="AH21" s="100"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <conditionalFormatting sqref="B8:B21">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
@@ -3740,7 +3639,7 @@
       <selection pane="topRight" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.86"/>
   </cols>
@@ -3807,10 +3706,10 @@
       <c r="C7" s="96" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="117" t="s">
+      <c r="D7" s="108" t="s">
         <v>86</v>
       </c>
-      <c r="E7" s="117" t="s">
+      <c r="E7" s="108" t="s">
         <v>87</v>
       </c>
       <c r="F7" s="96" t="s">
@@ -3822,7 +3721,7 @@
       <c r="H7" s="97" t="s">
         <v>108</v>
       </c>
-      <c r="I7" s="118" t="s">
+      <c r="I7" s="109" t="s">
         <v>109</v>
       </c>
       <c r="J7" s="97" t="s">
@@ -3840,7 +3739,7 @@
       <c r="N7" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="O7" s="119" t="s">
+      <c r="O7" s="110" t="s">
         <v>115</v>
       </c>
       <c r="P7" s="97" t="s">
@@ -3860,298 +3759,298 @@
       </c>
     </row>
     <row r="8" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="100"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="101"/>
-      <c r="G8" s="103"/>
-      <c r="H8" s="104"/>
-      <c r="I8" s="104"/>
-      <c r="J8" s="104"/>
-      <c r="K8" s="104"/>
-      <c r="L8" s="104"/>
-      <c r="M8" s="104"/>
-      <c r="N8" s="104"/>
-      <c r="O8" s="103"/>
-      <c r="P8" s="104"/>
-      <c r="Q8" s="101"/>
-      <c r="R8" s="104"/>
-      <c r="S8" s="104"/>
-      <c r="T8" s="104"/>
+      <c r="B8" s="111"/>
+      <c r="C8" s="112"/>
+      <c r="D8" s="112"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="112"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="113"/>
+      <c r="I8" s="113"/>
+      <c r="J8" s="113"/>
+      <c r="K8" s="113"/>
+      <c r="L8" s="113"/>
+      <c r="M8" s="113"/>
+      <c r="N8" s="113"/>
+      <c r="O8" s="111"/>
+      <c r="P8" s="113"/>
+      <c r="Q8" s="112"/>
+      <c r="R8" s="113"/>
+      <c r="S8" s="113"/>
+      <c r="T8" s="113"/>
     </row>
     <row r="9" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="100"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="102"/>
-      <c r="E9" s="102"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="103"/>
-      <c r="H9" s="104"/>
-      <c r="I9" s="104"/>
-      <c r="J9" s="104"/>
-      <c r="K9" s="104"/>
-      <c r="L9" s="104"/>
-      <c r="M9" s="104"/>
-      <c r="N9" s="104"/>
-      <c r="O9" s="103"/>
-      <c r="P9" s="104"/>
-      <c r="Q9" s="101"/>
-      <c r="R9" s="104"/>
-      <c r="S9" s="104"/>
-      <c r="T9" s="104"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="112"/>
+      <c r="D9" s="112"/>
+      <c r="E9" s="112"/>
+      <c r="F9" s="112"/>
+      <c r="G9" s="111"/>
+      <c r="H9" s="113"/>
+      <c r="I9" s="113"/>
+      <c r="J9" s="113"/>
+      <c r="K9" s="113"/>
+      <c r="L9" s="113"/>
+      <c r="M9" s="113"/>
+      <c r="N9" s="113"/>
+      <c r="O9" s="111"/>
+      <c r="P9" s="113"/>
+      <c r="Q9" s="112"/>
+      <c r="R9" s="113"/>
+      <c r="S9" s="113"/>
+      <c r="T9" s="113"/>
     </row>
     <row r="10" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="100"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="102"/>
-      <c r="E10" s="102"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="103"/>
-      <c r="H10" s="104"/>
-      <c r="I10" s="104"/>
-      <c r="J10" s="104"/>
-      <c r="K10" s="104"/>
-      <c r="L10" s="104"/>
-      <c r="M10" s="104"/>
-      <c r="N10" s="104"/>
-      <c r="O10" s="103"/>
-      <c r="P10" s="104"/>
-      <c r="Q10" s="101"/>
-      <c r="R10" s="104"/>
-      <c r="S10" s="104"/>
-      <c r="T10" s="104"/>
+      <c r="B10" s="111"/>
+      <c r="C10" s="112"/>
+      <c r="D10" s="112"/>
+      <c r="E10" s="112"/>
+      <c r="F10" s="112"/>
+      <c r="G10" s="111"/>
+      <c r="H10" s="113"/>
+      <c r="I10" s="113"/>
+      <c r="J10" s="113"/>
+      <c r="K10" s="113"/>
+      <c r="L10" s="113"/>
+      <c r="M10" s="113"/>
+      <c r="N10" s="113"/>
+      <c r="O10" s="111"/>
+      <c r="P10" s="113"/>
+      <c r="Q10" s="112"/>
+      <c r="R10" s="113"/>
+      <c r="S10" s="113"/>
+      <c r="T10" s="113"/>
     </row>
     <row r="11" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="100"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="103"/>
-      <c r="H11" s="104"/>
-      <c r="I11" s="104"/>
-      <c r="J11" s="104"/>
-      <c r="K11" s="104"/>
-      <c r="L11" s="104"/>
-      <c r="M11" s="104"/>
-      <c r="N11" s="104"/>
-      <c r="O11" s="103"/>
-      <c r="P11" s="104"/>
-      <c r="Q11" s="101"/>
-      <c r="R11" s="104"/>
-      <c r="S11" s="104"/>
-      <c r="T11" s="104"/>
+      <c r="B11" s="111"/>
+      <c r="C11" s="112"/>
+      <c r="D11" s="112"/>
+      <c r="E11" s="112"/>
+      <c r="F11" s="112"/>
+      <c r="G11" s="111"/>
+      <c r="H11" s="113"/>
+      <c r="I11" s="113"/>
+      <c r="J11" s="113"/>
+      <c r="K11" s="113"/>
+      <c r="L11" s="113"/>
+      <c r="M11" s="113"/>
+      <c r="N11" s="113"/>
+      <c r="O11" s="111"/>
+      <c r="P11" s="113"/>
+      <c r="Q11" s="112"/>
+      <c r="R11" s="113"/>
+      <c r="S11" s="113"/>
+      <c r="T11" s="113"/>
     </row>
     <row r="12" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="100"/>
-      <c r="C12" s="101"/>
-      <c r="D12" s="102"/>
-      <c r="E12" s="102"/>
-      <c r="F12" s="101"/>
-      <c r="G12" s="103"/>
-      <c r="H12" s="104"/>
-      <c r="I12" s="104"/>
-      <c r="J12" s="104"/>
-      <c r="K12" s="104"/>
-      <c r="L12" s="104"/>
-      <c r="M12" s="104"/>
-      <c r="N12" s="104"/>
-      <c r="O12" s="103"/>
-      <c r="P12" s="104"/>
-      <c r="Q12" s="101"/>
-      <c r="R12" s="104"/>
-      <c r="S12" s="104"/>
-      <c r="T12" s="104"/>
+      <c r="B12" s="111"/>
+      <c r="C12" s="112"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="112"/>
+      <c r="F12" s="112"/>
+      <c r="G12" s="111"/>
+      <c r="H12" s="113"/>
+      <c r="I12" s="113"/>
+      <c r="J12" s="113"/>
+      <c r="K12" s="113"/>
+      <c r="L12" s="113"/>
+      <c r="M12" s="113"/>
+      <c r="N12" s="113"/>
+      <c r="O12" s="111"/>
+      <c r="P12" s="113"/>
+      <c r="Q12" s="112"/>
+      <c r="R12" s="113"/>
+      <c r="S12" s="113"/>
+      <c r="T12" s="113"/>
     </row>
     <row r="13" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="100"/>
-      <c r="C13" s="101"/>
-      <c r="D13" s="102"/>
-      <c r="E13" s="102"/>
-      <c r="F13" s="101"/>
-      <c r="G13" s="103"/>
-      <c r="H13" s="104"/>
-      <c r="I13" s="104"/>
-      <c r="J13" s="104"/>
-      <c r="K13" s="104"/>
-      <c r="L13" s="104"/>
-      <c r="M13" s="104"/>
-      <c r="N13" s="104"/>
-      <c r="O13" s="103"/>
-      <c r="P13" s="104"/>
-      <c r="Q13" s="101"/>
-      <c r="R13" s="104"/>
-      <c r="S13" s="104"/>
-      <c r="T13" s="104"/>
+      <c r="B13" s="111"/>
+      <c r="C13" s="112"/>
+      <c r="D13" s="112"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="112"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="113"/>
+      <c r="I13" s="113"/>
+      <c r="J13" s="113"/>
+      <c r="K13" s="113"/>
+      <c r="L13" s="113"/>
+      <c r="M13" s="113"/>
+      <c r="N13" s="113"/>
+      <c r="O13" s="111"/>
+      <c r="P13" s="113"/>
+      <c r="Q13" s="112"/>
+      <c r="R13" s="113"/>
+      <c r="S13" s="113"/>
+      <c r="T13" s="113"/>
     </row>
     <row r="14" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="100"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="102"/>
-      <c r="E14" s="102"/>
-      <c r="F14" s="101"/>
-      <c r="G14" s="103"/>
-      <c r="H14" s="104"/>
-      <c r="I14" s="104"/>
-      <c r="J14" s="104"/>
-      <c r="K14" s="104"/>
-      <c r="L14" s="104"/>
-      <c r="M14" s="104"/>
-      <c r="N14" s="104"/>
-      <c r="O14" s="103"/>
-      <c r="P14" s="104"/>
-      <c r="Q14" s="101"/>
-      <c r="R14" s="104"/>
-      <c r="S14" s="104"/>
-      <c r="T14" s="104"/>
+      <c r="B14" s="111"/>
+      <c r="C14" s="112"/>
+      <c r="D14" s="112"/>
+      <c r="E14" s="112"/>
+      <c r="F14" s="112"/>
+      <c r="G14" s="111"/>
+      <c r="H14" s="113"/>
+      <c r="I14" s="113"/>
+      <c r="J14" s="113"/>
+      <c r="K14" s="113"/>
+      <c r="L14" s="113"/>
+      <c r="M14" s="113"/>
+      <c r="N14" s="113"/>
+      <c r="O14" s="111"/>
+      <c r="P14" s="113"/>
+      <c r="Q14" s="112"/>
+      <c r="R14" s="113"/>
+      <c r="S14" s="113"/>
+      <c r="T14" s="113"/>
     </row>
     <row r="15" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="100"/>
-      <c r="C15" s="101"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="102"/>
-      <c r="F15" s="101"/>
-      <c r="G15" s="103"/>
-      <c r="H15" s="104"/>
-      <c r="I15" s="104"/>
-      <c r="J15" s="104"/>
-      <c r="K15" s="104"/>
-      <c r="L15" s="104"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="104"/>
-      <c r="O15" s="103"/>
-      <c r="P15" s="104"/>
-      <c r="Q15" s="101"/>
-      <c r="R15" s="104"/>
-      <c r="S15" s="104"/>
-      <c r="T15" s="104"/>
+      <c r="B15" s="111"/>
+      <c r="C15" s="112"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="112"/>
+      <c r="F15" s="112"/>
+      <c r="G15" s="111"/>
+      <c r="H15" s="113"/>
+      <c r="I15" s="113"/>
+      <c r="J15" s="113"/>
+      <c r="K15" s="113"/>
+      <c r="L15" s="113"/>
+      <c r="M15" s="113"/>
+      <c r="N15" s="113"/>
+      <c r="O15" s="111"/>
+      <c r="P15" s="113"/>
+      <c r="Q15" s="112"/>
+      <c r="R15" s="113"/>
+      <c r="S15" s="113"/>
+      <c r="T15" s="113"/>
     </row>
     <row r="16" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="100"/>
-      <c r="C16" s="101"/>
-      <c r="D16" s="102"/>
-      <c r="E16" s="102"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="103"/>
-      <c r="H16" s="104"/>
-      <c r="I16" s="104"/>
-      <c r="J16" s="104"/>
-      <c r="K16" s="104"/>
-      <c r="L16" s="104"/>
-      <c r="M16" s="104"/>
-      <c r="N16" s="104"/>
-      <c r="O16" s="103"/>
-      <c r="P16" s="104"/>
-      <c r="Q16" s="101"/>
-      <c r="R16" s="104"/>
-      <c r="S16" s="104"/>
-      <c r="T16" s="104"/>
+      <c r="B16" s="111"/>
+      <c r="C16" s="112"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="112"/>
+      <c r="F16" s="112"/>
+      <c r="G16" s="111"/>
+      <c r="H16" s="113"/>
+      <c r="I16" s="113"/>
+      <c r="J16" s="113"/>
+      <c r="K16" s="113"/>
+      <c r="L16" s="113"/>
+      <c r="M16" s="113"/>
+      <c r="N16" s="113"/>
+      <c r="O16" s="111"/>
+      <c r="P16" s="113"/>
+      <c r="Q16" s="112"/>
+      <c r="R16" s="113"/>
+      <c r="S16" s="113"/>
+      <c r="T16" s="113"/>
     </row>
     <row r="17" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="100"/>
-      <c r="C17" s="101"/>
-      <c r="D17" s="102"/>
-      <c r="E17" s="102"/>
-      <c r="F17" s="101"/>
-      <c r="G17" s="103"/>
-      <c r="H17" s="104"/>
-      <c r="I17" s="104"/>
-      <c r="J17" s="104"/>
-      <c r="K17" s="104"/>
-      <c r="L17" s="104"/>
-      <c r="M17" s="104"/>
-      <c r="N17" s="104"/>
-      <c r="O17" s="103"/>
-      <c r="P17" s="104"/>
-      <c r="Q17" s="101"/>
-      <c r="R17" s="104"/>
-      <c r="S17" s="104"/>
-      <c r="T17" s="104"/>
+      <c r="B17" s="111"/>
+      <c r="C17" s="112"/>
+      <c r="D17" s="112"/>
+      <c r="E17" s="112"/>
+      <c r="F17" s="112"/>
+      <c r="G17" s="111"/>
+      <c r="H17" s="113"/>
+      <c r="I17" s="113"/>
+      <c r="J17" s="113"/>
+      <c r="K17" s="113"/>
+      <c r="L17" s="113"/>
+      <c r="M17" s="113"/>
+      <c r="N17" s="113"/>
+      <c r="O17" s="111"/>
+      <c r="P17" s="113"/>
+      <c r="Q17" s="112"/>
+      <c r="R17" s="113"/>
+      <c r="S17" s="113"/>
+      <c r="T17" s="113"/>
     </row>
     <row r="18" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="100"/>
-      <c r="C18" s="101"/>
-      <c r="D18" s="102"/>
-      <c r="E18" s="102"/>
-      <c r="F18" s="101"/>
-      <c r="G18" s="103"/>
-      <c r="H18" s="104"/>
-      <c r="I18" s="104"/>
-      <c r="J18" s="104"/>
-      <c r="K18" s="104"/>
-      <c r="L18" s="104"/>
-      <c r="M18" s="104"/>
-      <c r="N18" s="104"/>
-      <c r="O18" s="103"/>
-      <c r="P18" s="104"/>
-      <c r="Q18" s="101"/>
-      <c r="R18" s="104"/>
-      <c r="S18" s="104"/>
-      <c r="T18" s="104"/>
+      <c r="B18" s="111"/>
+      <c r="C18" s="112"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="112"/>
+      <c r="G18" s="111"/>
+      <c r="H18" s="113"/>
+      <c r="I18" s="113"/>
+      <c r="J18" s="113"/>
+      <c r="K18" s="113"/>
+      <c r="L18" s="113"/>
+      <c r="M18" s="113"/>
+      <c r="N18" s="113"/>
+      <c r="O18" s="111"/>
+      <c r="P18" s="113"/>
+      <c r="Q18" s="112"/>
+      <c r="R18" s="113"/>
+      <c r="S18" s="113"/>
+      <c r="T18" s="113"/>
     </row>
     <row r="19" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="100"/>
-      <c r="C19" s="101"/>
-      <c r="D19" s="102"/>
-      <c r="E19" s="102"/>
-      <c r="F19" s="101"/>
-      <c r="G19" s="103"/>
-      <c r="H19" s="104"/>
-      <c r="I19" s="104"/>
-      <c r="J19" s="104"/>
-      <c r="K19" s="104"/>
-      <c r="L19" s="104"/>
-      <c r="M19" s="104"/>
-      <c r="N19" s="104"/>
-      <c r="O19" s="103"/>
-      <c r="P19" s="104"/>
-      <c r="Q19" s="101"/>
-      <c r="R19" s="104"/>
-      <c r="S19" s="104"/>
-      <c r="T19" s="104"/>
+      <c r="B19" s="111"/>
+      <c r="C19" s="112"/>
+      <c r="D19" s="112"/>
+      <c r="E19" s="112"/>
+      <c r="F19" s="112"/>
+      <c r="G19" s="111"/>
+      <c r="H19" s="113"/>
+      <c r="I19" s="113"/>
+      <c r="J19" s="113"/>
+      <c r="K19" s="113"/>
+      <c r="L19" s="113"/>
+      <c r="M19" s="113"/>
+      <c r="N19" s="113"/>
+      <c r="O19" s="111"/>
+      <c r="P19" s="113"/>
+      <c r="Q19" s="112"/>
+      <c r="R19" s="113"/>
+      <c r="S19" s="113"/>
+      <c r="T19" s="113"/>
     </row>
     <row r="20" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="100"/>
-      <c r="C20" s="101"/>
-      <c r="D20" s="102"/>
-      <c r="E20" s="102"/>
-      <c r="F20" s="101"/>
-      <c r="G20" s="103"/>
-      <c r="H20" s="104"/>
-      <c r="I20" s="104"/>
-      <c r="J20" s="104"/>
-      <c r="K20" s="104"/>
-      <c r="L20" s="104"/>
-      <c r="M20" s="104"/>
-      <c r="N20" s="104"/>
-      <c r="O20" s="103"/>
-      <c r="P20" s="104"/>
-      <c r="Q20" s="101"/>
-      <c r="R20" s="104"/>
-      <c r="S20" s="104"/>
-      <c r="T20" s="104"/>
+      <c r="B20" s="111"/>
+      <c r="C20" s="112"/>
+      <c r="D20" s="112"/>
+      <c r="E20" s="112"/>
+      <c r="F20" s="112"/>
+      <c r="G20" s="111"/>
+      <c r="H20" s="113"/>
+      <c r="I20" s="113"/>
+      <c r="J20" s="113"/>
+      <c r="K20" s="113"/>
+      <c r="L20" s="113"/>
+      <c r="M20" s="113"/>
+      <c r="N20" s="113"/>
+      <c r="O20" s="111"/>
+      <c r="P20" s="113"/>
+      <c r="Q20" s="112"/>
+      <c r="R20" s="113"/>
+      <c r="S20" s="113"/>
+      <c r="T20" s="113"/>
     </row>
     <row r="21" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="100"/>
-      <c r="C21" s="101"/>
-      <c r="D21" s="102"/>
-      <c r="E21" s="102"/>
-      <c r="F21" s="101"/>
-      <c r="G21" s="103"/>
-      <c r="H21" s="104"/>
-      <c r="I21" s="104"/>
-      <c r="J21" s="104"/>
-      <c r="K21" s="104"/>
-      <c r="L21" s="104"/>
-      <c r="M21" s="104"/>
-      <c r="N21" s="104"/>
-      <c r="O21" s="103"/>
-      <c r="P21" s="104"/>
-      <c r="Q21" s="101"/>
-      <c r="R21" s="104"/>
-      <c r="S21" s="104"/>
-      <c r="T21" s="104"/>
+      <c r="B21" s="111"/>
+      <c r="C21" s="112"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="112"/>
+      <c r="F21" s="112"/>
+      <c r="G21" s="111"/>
+      <c r="H21" s="113"/>
+      <c r="I21" s="113"/>
+      <c r="J21" s="113"/>
+      <c r="K21" s="113"/>
+      <c r="L21" s="113"/>
+      <c r="M21" s="113"/>
+      <c r="N21" s="113"/>
+      <c r="O21" s="111"/>
+      <c r="P21" s="113"/>
+      <c r="Q21" s="112"/>
+      <c r="R21" s="113"/>
+      <c r="S21" s="113"/>
+      <c r="T21" s="113"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B8:B21">
@@ -4181,7 +4080,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.85"/>
@@ -4202,25 +4101,25 @@
       <c r="J4" s="89"/>
     </row>
     <row r="5" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="120" t="s">
+      <c r="B5" s="114" t="s">
         <v>116</v>
       </c>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="120"/>
-      <c r="G5" s="120"/>
-      <c r="H5" s="120"/>
-      <c r="I5" s="120"/>
-      <c r="J5" s="120"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="120"/>
+      <c r="C5" s="114"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="114"/>
+      <c r="G5" s="114"/>
+      <c r="H5" s="114"/>
+      <c r="I5" s="114"/>
+      <c r="J5" s="114"/>
+      <c r="K5" s="114"/>
+      <c r="L5" s="114"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J6" s="89"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" s="121" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="115" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0"/>
       <c r="C8" s="0"/>
       <c r="D8" s="0"/>
@@ -4240,7 +4139,7 @@
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" s="121" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="115" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0"/>
       <c r="C15" s="0"/>
       <c r="D15" s="0"/>
@@ -4284,112 +4183,112 @@
   <dimension ref="B3:I12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="116" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="122"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
-      <c r="G3" s="122"/>
-      <c r="H3" s="122"/>
-      <c r="I3" s="122"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="116"/>
+      <c r="F3" s="116"/>
+      <c r="G3" s="116"/>
+      <c r="H3" s="116"/>
+      <c r="I3" s="116"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="122"/>
-      <c r="C4" s="122"/>
-      <c r="D4" s="122"/>
-      <c r="E4" s="122"/>
-      <c r="F4" s="122"/>
-      <c r="G4" s="122"/>
-      <c r="H4" s="122"/>
-      <c r="I4" s="122"/>
+      <c r="B4" s="116"/>
+      <c r="C4" s="116"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
+      <c r="F4" s="116"/>
+      <c r="G4" s="116"/>
+      <c r="H4" s="116"/>
+      <c r="I4" s="116"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="122"/>
-      <c r="C5" s="122"/>
-      <c r="D5" s="122"/>
-      <c r="E5" s="122"/>
-      <c r="F5" s="122"/>
-      <c r="G5" s="122"/>
-      <c r="H5" s="122"/>
-      <c r="I5" s="122"/>
+      <c r="B5" s="116"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="116"/>
+      <c r="E5" s="116"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="116"/>
+      <c r="H5" s="116"/>
+      <c r="I5" s="116"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="122"/>
-      <c r="C6" s="122"/>
-      <c r="D6" s="122"/>
-      <c r="E6" s="122"/>
-      <c r="F6" s="122"/>
-      <c r="G6" s="122"/>
-      <c r="H6" s="122"/>
-      <c r="I6" s="122"/>
+      <c r="B6" s="116"/>
+      <c r="C6" s="116"/>
+      <c r="D6" s="116"/>
+      <c r="E6" s="116"/>
+      <c r="F6" s="116"/>
+      <c r="G6" s="116"/>
+      <c r="H6" s="116"/>
+      <c r="I6" s="116"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="122"/>
-      <c r="C7" s="122"/>
-      <c r="D7" s="122"/>
-      <c r="E7" s="122"/>
-      <c r="F7" s="122"/>
-      <c r="G7" s="122"/>
-      <c r="H7" s="122"/>
-      <c r="I7" s="122"/>
+      <c r="B7" s="116"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
+      <c r="G7" s="116"/>
+      <c r="H7" s="116"/>
+      <c r="I7" s="116"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="122"/>
-      <c r="C8" s="122"/>
-      <c r="D8" s="122"/>
-      <c r="E8" s="122"/>
-      <c r="F8" s="122"/>
-      <c r="G8" s="122"/>
-      <c r="H8" s="122"/>
-      <c r="I8" s="122"/>
+      <c r="B8" s="116"/>
+      <c r="C8" s="116"/>
+      <c r="D8" s="116"/>
+      <c r="E8" s="116"/>
+      <c r="F8" s="116"/>
+      <c r="G8" s="116"/>
+      <c r="H8" s="116"/>
+      <c r="I8" s="116"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="122"/>
-      <c r="C9" s="122"/>
-      <c r="D9" s="122"/>
-      <c r="E9" s="122"/>
-      <c r="F9" s="122"/>
-      <c r="G9" s="122"/>
-      <c r="H9" s="122"/>
-      <c r="I9" s="122"/>
+      <c r="B9" s="116"/>
+      <c r="C9" s="116"/>
+      <c r="D9" s="116"/>
+      <c r="E9" s="116"/>
+      <c r="F9" s="116"/>
+      <c r="G9" s="116"/>
+      <c r="H9" s="116"/>
+      <c r="I9" s="116"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="122"/>
-      <c r="C10" s="122"/>
-      <c r="D10" s="122"/>
-      <c r="E10" s="122"/>
-      <c r="F10" s="122"/>
-      <c r="G10" s="122"/>
-      <c r="H10" s="122"/>
-      <c r="I10" s="122"/>
+      <c r="B10" s="116"/>
+      <c r="C10" s="116"/>
+      <c r="D10" s="116"/>
+      <c r="E10" s="116"/>
+      <c r="F10" s="116"/>
+      <c r="G10" s="116"/>
+      <c r="H10" s="116"/>
+      <c r="I10" s="116"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="122"/>
-      <c r="C11" s="122"/>
-      <c r="D11" s="122"/>
-      <c r="E11" s="122"/>
-      <c r="F11" s="122"/>
-      <c r="G11" s="122"/>
-      <c r="H11" s="122"/>
-      <c r="I11" s="122"/>
+      <c r="B11" s="116"/>
+      <c r="C11" s="116"/>
+      <c r="D11" s="116"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="116"/>
+      <c r="G11" s="116"/>
+      <c r="H11" s="116"/>
+      <c r="I11" s="116"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="122"/>
-      <c r="C12" s="122"/>
-      <c r="D12" s="122"/>
-      <c r="E12" s="122"/>
-      <c r="F12" s="122"/>
-      <c r="G12" s="122"/>
-      <c r="H12" s="122"/>
-      <c r="I12" s="122"/>
+      <c r="B12" s="116"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="116"/>
+      <c r="G12" s="116"/>
+      <c r="H12" s="116"/>
+      <c r="I12" s="116"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4410,560 +4309,546 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="123" width="3.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="123" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="123" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="123" width="13.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="123" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="123" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="123" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="123" width="8.28"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="9" style="123" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="123" width="11.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="12" style="123" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="123" width="36.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="15" style="123" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="117" width="3.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="117" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="117" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="117" width="13.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="117" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="117" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="117" width="13.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="117" width="8.28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="9" style="117" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="117" width="11.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="12" style="117" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="117" width="36.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="15" style="117" width="11.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="124"/>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124"/>
-      <c r="I1" s="124"/>
-      <c r="J1" s="124"/>
-      <c r="K1" s="124"/>
-      <c r="L1" s="124"/>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
+      <c r="A1" s="118"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="118"/>
     </row>
     <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="124"/>
-      <c r="B2" s="125" t="s">
+      <c r="A2" s="118"/>
+      <c r="B2" s="119" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
-      <c r="G2" s="125"/>
-      <c r="H2" s="125"/>
-      <c r="I2" s="125"/>
-      <c r="J2" s="125"/>
-      <c r="K2" s="125"/>
-      <c r="L2" s="125"/>
-      <c r="M2" s="125"/>
-      <c r="N2" s="125"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="119"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="119"/>
+      <c r="M2" s="119"/>
+      <c r="N2" s="119"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="124"/>
-      <c r="B3" s="124"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
-      <c r="F3" s="124"/>
-      <c r="G3" s="124"/>
-      <c r="H3" s="124"/>
-      <c r="I3" s="124"/>
-      <c r="J3" s="124"/>
-      <c r="K3" s="124"/>
-      <c r="L3" s="124"/>
-      <c r="M3" s="124"/>
-      <c r="N3" s="124"/>
+      <c r="A3" s="118"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="118"/>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="124"/>
-      <c r="B4" s="126" t="s">
+      <c r="A4" s="118"/>
+      <c r="B4" s="120" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="126"/>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
-      <c r="F4" s="126"/>
-      <c r="G4" s="126"/>
-      <c r="H4" s="126"/>
-      <c r="I4" s="126"/>
-      <c r="J4" s="126"/>
-      <c r="K4" s="126"/>
-      <c r="L4" s="126"/>
-      <c r="M4" s="126"/>
-      <c r="N4" s="126"/>
+      <c r="C4" s="120"/>
+      <c r="D4" s="120"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="120"/>
+      <c r="G4" s="120"/>
+      <c r="H4" s="120"/>
+      <c r="I4" s="120"/>
+      <c r="J4" s="120"/>
+      <c r="K4" s="120"/>
+      <c r="L4" s="120"/>
+      <c r="M4" s="120"/>
+      <c r="N4" s="120"/>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="124"/>
-      <c r="B5" s="127"/>
-      <c r="C5" s="127"/>
-      <c r="D5" s="127"/>
-      <c r="E5" s="127"/>
-      <c r="F5" s="127"/>
-      <c r="G5" s="127"/>
-      <c r="H5" s="127"/>
-      <c r="I5" s="127"/>
-      <c r="J5" s="127"/>
-      <c r="K5" s="127"/>
-      <c r="L5" s="127"/>
-      <c r="M5" s="127"/>
-      <c r="N5" s="127"/>
+      <c r="A5" s="118"/>
+      <c r="B5" s="121"/>
+      <c r="C5" s="121"/>
+      <c r="D5" s="121"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="121"/>
+      <c r="I5" s="121"/>
+      <c r="J5" s="121"/>
+      <c r="K5" s="121"/>
+      <c r="L5" s="121"/>
+      <c r="M5" s="121"/>
+      <c r="N5" s="121"/>
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="124"/>
-      <c r="B6" s="127" t="s">
+      <c r="A6" s="118"/>
+      <c r="B6" s="121" t="s">
         <v>120</v>
       </c>
-      <c r="C6" s="127"/>
-      <c r="D6" s="127"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="127"/>
-      <c r="J6" s="127"/>
-      <c r="K6" s="127"/>
-      <c r="L6" s="127"/>
-      <c r="M6" s="127"/>
-      <c r="N6" s="127"/>
+      <c r="C6" s="121"/>
+      <c r="D6" s="121"/>
+      <c r="E6" s="121"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="121"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="121"/>
+      <c r="K6" s="121"/>
+      <c r="L6" s="121"/>
+      <c r="M6" s="121"/>
+      <c r="N6" s="121"/>
     </row>
     <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="124"/>
-      <c r="B7" s="127"/>
-      <c r="C7" s="127"/>
-      <c r="D7" s="127"/>
-      <c r="E7" s="127"/>
-      <c r="F7" s="127"/>
-      <c r="G7" s="127"/>
-      <c r="H7" s="127"/>
-      <c r="I7" s="127"/>
-      <c r="J7" s="127"/>
-      <c r="K7" s="127"/>
-      <c r="L7" s="127"/>
-      <c r="M7" s="127"/>
-      <c r="N7" s="127"/>
+      <c r="A7" s="118"/>
+      <c r="B7" s="121"/>
+      <c r="C7" s="121"/>
+      <c r="D7" s="121"/>
+      <c r="E7" s="121"/>
+      <c r="F7" s="121"/>
+      <c r="G7" s="121"/>
+      <c r="H7" s="121"/>
+      <c r="I7" s="121"/>
+      <c r="J7" s="121"/>
+      <c r="K7" s="121"/>
+      <c r="L7" s="121"/>
+      <c r="M7" s="121"/>
+      <c r="N7" s="121"/>
     </row>
     <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="124"/>
-      <c r="B8" s="126" t="s">
+      <c r="A8" s="118"/>
+      <c r="B8" s="120" t="s">
         <v>121</v>
       </c>
-      <c r="C8" s="126"/>
-      <c r="D8" s="126"/>
-      <c r="E8" s="126"/>
-      <c r="F8" s="126"/>
-      <c r="G8" s="126"/>
-      <c r="H8" s="126"/>
-      <c r="I8" s="126"/>
-      <c r="J8" s="126"/>
-      <c r="K8" s="126"/>
-      <c r="L8" s="126"/>
-      <c r="M8" s="126"/>
-      <c r="N8" s="126"/>
+      <c r="C8" s="120"/>
+      <c r="D8" s="120"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="120"/>
+      <c r="G8" s="120"/>
+      <c r="H8" s="120"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="120"/>
+      <c r="K8" s="120"/>
+      <c r="L8" s="120"/>
+      <c r="M8" s="120"/>
+      <c r="N8" s="120"/>
     </row>
     <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="124"/>
-      <c r="B9" s="127"/>
-      <c r="C9" s="127"/>
-      <c r="D9" s="127"/>
-      <c r="E9" s="127"/>
-      <c r="F9" s="127"/>
-      <c r="G9" s="127"/>
-      <c r="H9" s="127"/>
-      <c r="I9" s="127"/>
-      <c r="J9" s="127"/>
-      <c r="K9" s="127"/>
-      <c r="L9" s="127"/>
-      <c r="M9" s="127"/>
-      <c r="N9" s="127"/>
+      <c r="A9" s="118"/>
+      <c r="B9" s="121"/>
+      <c r="C9" s="121"/>
+      <c r="D9" s="121"/>
+      <c r="E9" s="121"/>
+      <c r="F9" s="121"/>
+      <c r="G9" s="121"/>
+      <c r="H9" s="121"/>
+      <c r="I9" s="121"/>
+      <c r="J9" s="121"/>
+      <c r="K9" s="121"/>
+      <c r="L9" s="121"/>
+      <c r="M9" s="121"/>
+      <c r="N9" s="121"/>
     </row>
     <row r="10" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="124"/>
-      <c r="B10" s="128" t="s">
+      <c r="A10" s="118"/>
+      <c r="B10" s="122" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="128"/>
-      <c r="D10" s="128"/>
-      <c r="E10" s="128"/>
-      <c r="F10" s="128"/>
-      <c r="G10" s="128"/>
-      <c r="H10" s="128"/>
-      <c r="I10" s="128"/>
-      <c r="J10" s="128"/>
-      <c r="K10" s="128"/>
-      <c r="L10" s="128"/>
-      <c r="M10" s="128"/>
-      <c r="N10" s="128"/>
+      <c r="C10" s="122"/>
+      <c r="D10" s="122"/>
+      <c r="E10" s="122"/>
+      <c r="F10" s="122"/>
+      <c r="G10" s="122"/>
+      <c r="H10" s="122"/>
+      <c r="I10" s="122"/>
+      <c r="J10" s="122"/>
+      <c r="K10" s="122"/>
+      <c r="L10" s="122"/>
+      <c r="M10" s="122"/>
+      <c r="N10" s="122"/>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="124"/>
-      <c r="B11" s="127"/>
-      <c r="C11" s="127"/>
-      <c r="D11" s="127"/>
-      <c r="E11" s="127"/>
-      <c r="F11" s="127"/>
-      <c r="G11" s="127"/>
-      <c r="H11" s="127"/>
-      <c r="I11" s="127"/>
-      <c r="J11" s="129"/>
-      <c r="K11" s="127"/>
-      <c r="L11" s="127"/>
-      <c r="M11" s="127"/>
-      <c r="N11" s="127"/>
+      <c r="A11" s="118"/>
+      <c r="B11" s="121"/>
+      <c r="C11" s="121"/>
+      <c r="D11" s="121"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="121"/>
+      <c r="G11" s="121"/>
+      <c r="H11" s="121"/>
+      <c r="I11" s="121"/>
+      <c r="J11" s="123"/>
+      <c r="K11" s="121"/>
+      <c r="L11" s="121"/>
+      <c r="M11" s="121"/>
+      <c r="N11" s="121"/>
     </row>
     <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="124"/>
-      <c r="B12" s="126" t="s">
+      <c r="A12" s="118"/>
+      <c r="B12" s="120" t="s">
         <v>123</v>
       </c>
-      <c r="C12" s="126"/>
-      <c r="D12" s="126"/>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
-      <c r="G12" s="126"/>
-      <c r="H12" s="126"/>
-      <c r="I12" s="126"/>
-      <c r="J12" s="126"/>
-      <c r="K12" s="126"/>
-      <c r="L12" s="126"/>
-      <c r="M12" s="126"/>
-      <c r="N12" s="126"/>
+      <c r="C12" s="120"/>
+      <c r="D12" s="120"/>
+      <c r="E12" s="120"/>
+      <c r="F12" s="120"/>
+      <c r="G12" s="120"/>
+      <c r="H12" s="120"/>
+      <c r="I12" s="120"/>
+      <c r="J12" s="120"/>
+      <c r="K12" s="120"/>
+      <c r="L12" s="120"/>
+      <c r="M12" s="120"/>
+      <c r="N12" s="120"/>
     </row>
     <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="124"/>
-      <c r="B13" s="127"/>
-      <c r="C13" s="127"/>
-      <c r="D13" s="127"/>
-      <c r="E13" s="127"/>
-      <c r="F13" s="127"/>
-      <c r="G13" s="127"/>
-      <c r="H13" s="127"/>
-      <c r="I13" s="127"/>
-      <c r="J13" s="127"/>
-      <c r="K13" s="127"/>
-      <c r="L13" s="127"/>
-      <c r="M13" s="127"/>
-      <c r="N13" s="127"/>
+      <c r="A13" s="118"/>
+      <c r="B13" s="121"/>
+      <c r="C13" s="121"/>
+      <c r="D13" s="121"/>
+      <c r="E13" s="121"/>
+      <c r="F13" s="121"/>
+      <c r="G13" s="121"/>
+      <c r="H13" s="121"/>
+      <c r="I13" s="121"/>
+      <c r="J13" s="121"/>
+      <c r="K13" s="121"/>
+      <c r="L13" s="121"/>
+      <c r="M13" s="121"/>
+      <c r="N13" s="121"/>
     </row>
     <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="124"/>
-      <c r="B14" s="127" t="s">
+      <c r="A14" s="118"/>
+      <c r="B14" s="121" t="s">
         <v>124</v>
       </c>
-      <c r="C14" s="127"/>
-      <c r="D14" s="127"/>
-      <c r="E14" s="127"/>
-      <c r="F14" s="127"/>
-      <c r="G14" s="127"/>
-      <c r="H14" s="127"/>
-      <c r="I14" s="127"/>
-      <c r="J14" s="127"/>
-      <c r="K14" s="127"/>
-      <c r="L14" s="127"/>
-      <c r="M14" s="127"/>
-      <c r="N14" s="127"/>
+      <c r="C14" s="121"/>
+      <c r="D14" s="121"/>
+      <c r="E14" s="121"/>
+      <c r="F14" s="121"/>
+      <c r="G14" s="121"/>
+      <c r="H14" s="121"/>
+      <c r="I14" s="121"/>
+      <c r="J14" s="121"/>
+      <c r="K14" s="121"/>
+      <c r="L14" s="121"/>
+      <c r="M14" s="121"/>
+      <c r="N14" s="121"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="124"/>
-      <c r="B15" s="124"/>
-      <c r="C15" s="124"/>
-      <c r="D15" s="124"/>
-      <c r="E15" s="124"/>
-      <c r="F15" s="124"/>
-      <c r="G15" s="124"/>
-      <c r="H15" s="124"/>
-      <c r="I15" s="124"/>
-      <c r="J15" s="124"/>
-      <c r="K15" s="124"/>
-      <c r="L15" s="124"/>
-      <c r="M15" s="124"/>
-      <c r="N15" s="124"/>
+      <c r="A15" s="118"/>
+      <c r="B15" s="118"/>
+      <c r="C15" s="118"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="118"/>
+      <c r="F15" s="118"/>
+      <c r="G15" s="118"/>
+      <c r="H15" s="118"/>
+      <c r="I15" s="118"/>
+      <c r="J15" s="118"/>
+      <c r="K15" s="118"/>
+      <c r="L15" s="118"/>
+      <c r="M15" s="118"/>
+      <c r="N15" s="118"/>
     </row>
     <row r="16" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="130" t="s">
+      <c r="B16" s="124" t="s">
         <v>125</v>
       </c>
-      <c r="C16" s="130"/>
-      <c r="D16" s="130" t="s">
+      <c r="C16" s="124"/>
+      <c r="D16" s="124" t="s">
         <v>126</v>
       </c>
-      <c r="E16" s="130" t="s">
+      <c r="E16" s="124" t="s">
         <v>127</v>
       </c>
-      <c r="F16" s="130"/>
-      <c r="G16" s="131" t="s">
+      <c r="F16" s="124"/>
+      <c r="G16" s="125" t="s">
         <v>128</v>
       </c>
-      <c r="H16" s="131" t="s">
+      <c r="H16" s="125" t="s">
         <v>129</v>
       </c>
-      <c r="I16" s="130" t="s">
+      <c r="I16" s="124" t="s">
         <v>130</v>
       </c>
-      <c r="J16" s="130" t="s">
+      <c r="J16" s="124" t="s">
         <v>131</v>
       </c>
-      <c r="K16" s="131" t="s">
+      <c r="K16" s="125" t="s">
         <v>132</v>
       </c>
-      <c r="L16" s="130" t="s">
+      <c r="L16" s="124" t="s">
         <v>133</v>
       </c>
-      <c r="M16" s="130"/>
-      <c r="N16" s="130" t="s">
+      <c r="M16" s="124"/>
+      <c r="N16" s="124" t="s">
         <v>134</v>
       </c>
-      <c r="O16" s="123" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B17" s="126"/>
+      <c r="C17" s="126"/>
+      <c r="D17" s="127"/>
+      <c r="E17" s="126"/>
+      <c r="F17" s="126"/>
+      <c r="G17" s="127"/>
+      <c r="H17" s="127"/>
+      <c r="I17" s="127"/>
+      <c r="J17" s="127"/>
+      <c r="K17" s="127"/>
+      <c r="L17" s="127"/>
+      <c r="M17" s="127"/>
+      <c r="N17" s="127"/>
+    </row>
+    <row r="18" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B18" s="128"/>
+      <c r="C18" s="128"/>
+      <c r="D18" s="129"/>
+      <c r="E18" s="130"/>
+      <c r="F18" s="130"/>
+      <c r="G18" s="129"/>
+      <c r="H18" s="129"/>
+      <c r="I18" s="129"/>
+      <c r="J18" s="129"/>
+      <c r="K18" s="129"/>
+      <c r="L18" s="129"/>
+      <c r="M18" s="129"/>
+      <c r="N18" s="129"/>
+    </row>
+    <row r="19" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B19" s="128"/>
+      <c r="C19" s="128"/>
+      <c r="D19" s="129"/>
+      <c r="E19" s="130"/>
+      <c r="F19" s="130"/>
+      <c r="G19" s="129"/>
+      <c r="H19" s="129"/>
+      <c r="I19" s="129"/>
+      <c r="J19" s="129"/>
+      <c r="K19" s="129"/>
+      <c r="L19" s="129"/>
+      <c r="M19" s="129"/>
+      <c r="N19" s="129"/>
+    </row>
+    <row r="20" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B20" s="128"/>
+      <c r="C20" s="128"/>
+      <c r="D20" s="129"/>
+      <c r="E20" s="130"/>
+      <c r="F20" s="130"/>
+      <c r="G20" s="129"/>
+      <c r="H20" s="129"/>
+      <c r="I20" s="129"/>
+      <c r="J20" s="129"/>
+      <c r="K20" s="129"/>
+      <c r="L20" s="129"/>
+      <c r="M20" s="129"/>
+      <c r="N20" s="129"/>
+    </row>
+    <row r="21" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B21" s="128"/>
+      <c r="C21" s="128"/>
+      <c r="D21" s="129"/>
+      <c r="E21" s="130"/>
+      <c r="F21" s="130"/>
+      <c r="G21" s="129"/>
+      <c r="H21" s="129"/>
+      <c r="I21" s="129"/>
+      <c r="J21" s="129"/>
+      <c r="K21" s="129"/>
+      <c r="L21" s="129"/>
+      <c r="M21" s="129"/>
+      <c r="N21" s="129"/>
+    </row>
+    <row r="22" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B22" s="128"/>
+      <c r="C22" s="128"/>
+      <c r="D22" s="129"/>
+      <c r="E22" s="130"/>
+      <c r="F22" s="130"/>
+      <c r="G22" s="129"/>
+      <c r="H22" s="129"/>
+      <c r="I22" s="129"/>
+      <c r="J22" s="129"/>
+      <c r="K22" s="129"/>
+      <c r="L22" s="129"/>
+      <c r="M22" s="129"/>
+      <c r="N22" s="129"/>
+    </row>
+    <row r="24" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="131" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="132"/>
-      <c r="C17" s="132"/>
-      <c r="D17" s="133"/>
-      <c r="E17" s="132"/>
-      <c r="F17" s="132"/>
-      <c r="G17" s="133"/>
-      <c r="H17" s="133"/>
-      <c r="I17" s="133"/>
-      <c r="J17" s="133"/>
-      <c r="K17" s="133"/>
-      <c r="L17" s="133"/>
-      <c r="M17" s="133"/>
-      <c r="N17" s="133"/>
-    </row>
-    <row r="18" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="134"/>
-      <c r="C18" s="134"/>
-      <c r="D18" s="135"/>
-      <c r="E18" s="136"/>
-      <c r="F18" s="136"/>
-      <c r="G18" s="135"/>
-      <c r="H18" s="135"/>
-      <c r="I18" s="135"/>
-      <c r="J18" s="135"/>
-      <c r="K18" s="135"/>
-      <c r="L18" s="135"/>
-      <c r="M18" s="135"/>
-      <c r="N18" s="135"/>
-    </row>
-    <row r="19" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="134"/>
-      <c r="C19" s="134"/>
-      <c r="D19" s="135"/>
-      <c r="E19" s="136"/>
-      <c r="F19" s="136"/>
-      <c r="G19" s="135"/>
-      <c r="H19" s="135"/>
-      <c r="I19" s="135"/>
-      <c r="J19" s="135"/>
-      <c r="K19" s="135"/>
-      <c r="L19" s="135"/>
-      <c r="M19" s="135"/>
-      <c r="N19" s="135"/>
-    </row>
-    <row r="20" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="134"/>
-      <c r="C20" s="134"/>
-      <c r="D20" s="135"/>
-      <c r="E20" s="136"/>
-      <c r="F20" s="136"/>
-      <c r="G20" s="135"/>
-      <c r="H20" s="135"/>
-      <c r="I20" s="135"/>
-      <c r="J20" s="135"/>
-      <c r="K20" s="135"/>
-      <c r="L20" s="135"/>
-      <c r="M20" s="135"/>
-      <c r="N20" s="135"/>
-    </row>
-    <row r="21" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="134"/>
-      <c r="C21" s="134"/>
-      <c r="D21" s="135"/>
-      <c r="E21" s="136"/>
-      <c r="F21" s="136"/>
-      <c r="G21" s="135"/>
-      <c r="H21" s="135"/>
-      <c r="I21" s="135"/>
-      <c r="J21" s="135"/>
-      <c r="K21" s="135"/>
-      <c r="L21" s="135"/>
-      <c r="M21" s="135"/>
-      <c r="N21" s="135"/>
-    </row>
-    <row r="22" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="134"/>
-      <c r="C22" s="134"/>
-      <c r="D22" s="135"/>
-      <c r="E22" s="136"/>
-      <c r="F22" s="136"/>
-      <c r="G22" s="135"/>
-      <c r="H22" s="135"/>
-      <c r="I22" s="135"/>
-      <c r="J22" s="135"/>
-      <c r="K22" s="135"/>
-      <c r="L22" s="135"/>
-      <c r="M22" s="135"/>
-      <c r="N22" s="135"/>
-    </row>
-    <row r="24" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="137" t="s">
+      <c r="C24" s="131"/>
+      <c r="D24" s="131"/>
+      <c r="E24" s="131"/>
+      <c r="F24" s="131"/>
+      <c r="G24" s="131"/>
+      <c r="H24" s="131"/>
+      <c r="I24" s="131"/>
+      <c r="J24" s="131"/>
+      <c r="K24" s="131"/>
+      <c r="L24" s="131"/>
+      <c r="M24" s="131"/>
+      <c r="N24" s="131"/>
+    </row>
+    <row r="26" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B26" s="132" t="s">
         <v>136</v>
       </c>
-      <c r="C24" s="137"/>
-      <c r="D24" s="137"/>
-      <c r="E24" s="137"/>
-      <c r="F24" s="137"/>
-      <c r="G24" s="137"/>
-      <c r="H24" s="137"/>
-      <c r="I24" s="137"/>
-      <c r="J24" s="137"/>
-      <c r="K24" s="137"/>
-      <c r="L24" s="137"/>
-      <c r="M24" s="137"/>
-      <c r="N24" s="137"/>
-    </row>
-    <row r="26" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="138" t="s">
+      <c r="C26" s="132" t="s">
         <v>137</v>
       </c>
-      <c r="C26" s="138" t="s">
+      <c r="D26" s="132" t="s">
         <v>138</v>
       </c>
-      <c r="D26" s="138" t="s">
+      <c r="E26" s="132" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="132" t="s">
         <v>139</v>
       </c>
-      <c r="E26" s="138" t="s">
-        <v>89</v>
-      </c>
-      <c r="F26" s="138" t="s">
+      <c r="G26" s="133" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="133"/>
+      <c r="I26" s="133" t="s">
+        <v>60</v>
+      </c>
+      <c r="J26" s="133"/>
+      <c r="K26" s="133"/>
+      <c r="L26" s="133" t="s">
+        <v>61</v>
+      </c>
+      <c r="M26" s="133"/>
+      <c r="N26" s="133" t="s">
         <v>140</v>
       </c>
-      <c r="G26" s="139" t="s">
-        <v>58</v>
-      </c>
-      <c r="H26" s="139"/>
-      <c r="I26" s="139" t="s">
-        <v>60</v>
-      </c>
-      <c r="J26" s="139"/>
-      <c r="K26" s="139"/>
-      <c r="L26" s="139" t="s">
-        <v>61</v>
-      </c>
-      <c r="M26" s="139"/>
-      <c r="N26" s="139" t="s">
+      <c r="O26" s="134"/>
+    </row>
+    <row r="27" s="135" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B27" s="136"/>
+      <c r="C27" s="136"/>
+      <c r="D27" s="136"/>
+      <c r="E27" s="136"/>
+      <c r="F27" s="137"/>
+      <c r="G27" s="136"/>
+      <c r="H27" s="136"/>
+      <c r="I27" s="136"/>
+      <c r="J27" s="136"/>
+      <c r="K27" s="136"/>
+      <c r="L27" s="136"/>
+      <c r="M27" s="136"/>
+      <c r="N27" s="138"/>
+    </row>
+    <row r="29" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="139" t="s">
         <v>141</v>
       </c>
-      <c r="O26" s="123" t="s">
+      <c r="C29" s="139"/>
+      <c r="D29" s="139"/>
+      <c r="E29" s="139"/>
+      <c r="F29" s="139"/>
+      <c r="G29" s="139"/>
+      <c r="H29" s="139"/>
+      <c r="I29" s="139"/>
+      <c r="J29" s="139"/>
+      <c r="K29" s="139"/>
+      <c r="L29" s="139"/>
+      <c r="M29" s="139"/>
+      <c r="N29" s="139"/>
+    </row>
+    <row r="30" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B30" s="139"/>
+      <c r="C30" s="139"/>
+      <c r="D30" s="139"/>
+      <c r="E30" s="139"/>
+      <c r="F30" s="139"/>
+      <c r="G30" s="139"/>
+      <c r="H30" s="139"/>
+      <c r="I30" s="139"/>
+      <c r="J30" s="139"/>
+      <c r="K30" s="139"/>
+      <c r="L30" s="139"/>
+      <c r="M30" s="139"/>
+      <c r="N30" s="139"/>
+    </row>
+    <row r="31" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B31" s="140" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="27" s="140" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="141"/>
-      <c r="C27" s="141"/>
-      <c r="D27" s="141"/>
-      <c r="E27" s="141"/>
-      <c r="F27" s="142"/>
-      <c r="G27" s="141"/>
-      <c r="H27" s="141"/>
-      <c r="I27" s="141"/>
-      <c r="J27" s="141"/>
-      <c r="K27" s="141"/>
-      <c r="L27" s="141"/>
-      <c r="M27" s="141"/>
-      <c r="N27" s="143"/>
-    </row>
-    <row r="28" s="140" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="141"/>
-      <c r="C28" s="141"/>
-      <c r="D28" s="141"/>
-      <c r="E28" s="141"/>
-      <c r="F28" s="142"/>
-      <c r="G28" s="141"/>
-      <c r="H28" s="141"/>
-      <c r="I28" s="141"/>
-      <c r="J28" s="141"/>
-      <c r="K28" s="141"/>
-      <c r="L28" s="141"/>
-      <c r="M28" s="141"/>
-      <c r="N28" s="143"/>
-    </row>
-    <row r="29" s="140" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="141"/>
-      <c r="C29" s="141"/>
-      <c r="D29" s="141"/>
-      <c r="E29" s="141"/>
-      <c r="F29" s="142"/>
-      <c r="G29" s="141"/>
-      <c r="H29" s="141"/>
-      <c r="I29" s="141"/>
-      <c r="J29" s="141"/>
-      <c r="K29" s="141"/>
-      <c r="L29" s="141"/>
-      <c r="M29" s="141"/>
-      <c r="N29" s="143"/>
-    </row>
-    <row r="30" s="140" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="141"/>
-      <c r="C30" s="141"/>
-      <c r="D30" s="141"/>
-      <c r="E30" s="141"/>
-      <c r="F30" s="142"/>
-      <c r="G30" s="141"/>
-      <c r="H30" s="141"/>
-      <c r="I30" s="141"/>
-      <c r="J30" s="141"/>
-      <c r="K30" s="141"/>
-      <c r="L30" s="141"/>
-      <c r="M30" s="141"/>
-      <c r="N30" s="143"/>
-    </row>
-    <row r="31" s="140" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="141"/>
-      <c r="C31" s="141"/>
-      <c r="D31" s="141"/>
-      <c r="E31" s="141"/>
-      <c r="F31" s="142"/>
-      <c r="G31" s="141"/>
-      <c r="H31" s="141"/>
-      <c r="I31" s="141"/>
-      <c r="J31" s="141"/>
-      <c r="K31" s="141"/>
-      <c r="L31" s="141"/>
-      <c r="M31" s="141"/>
-      <c r="N31" s="143"/>
-    </row>
-    <row r="32" s="140" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="141"/>
-      <c r="C32" s="141"/>
-      <c r="D32" s="141"/>
-      <c r="E32" s="141"/>
-      <c r="F32" s="142"/>
-      <c r="G32" s="141"/>
-      <c r="H32" s="141"/>
-      <c r="I32" s="141"/>
-      <c r="J32" s="141"/>
-      <c r="K32" s="141"/>
-      <c r="L32" s="141"/>
-      <c r="M32" s="141"/>
-      <c r="N32" s="143"/>
-    </row>
-    <row r="33" s="140" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="141"/>
+      <c r="C31" s="140"/>
+      <c r="D31" s="140"/>
+      <c r="E31" s="140"/>
+      <c r="F31" s="140"/>
+      <c r="G31" s="140"/>
+      <c r="H31" s="140"/>
+      <c r="I31" s="140"/>
+      <c r="J31" s="140"/>
+      <c r="K31" s="140"/>
+      <c r="L31" s="140"/>
+      <c r="M31" s="140"/>
+      <c r="N31" s="140"/>
+    </row>
+    <row r="32" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B32" s="140"/>
+      <c r="C32" s="140"/>
+      <c r="D32" s="140"/>
+      <c r="E32" s="140"/>
+      <c r="F32" s="140"/>
+      <c r="G32" s="140"/>
+      <c r="H32" s="140"/>
+      <c r="I32" s="140"/>
+      <c r="J32" s="140"/>
+      <c r="K32" s="140"/>
+      <c r="L32" s="140"/>
+      <c r="M32" s="140"/>
+      <c r="N32" s="140"/>
+    </row>
+    <row r="33" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="141" t="s">
+        <v>143</v>
+      </c>
       <c r="C33" s="141"/>
       <c r="D33" s="141"/>
       <c r="E33" s="141"/>
-      <c r="F33" s="142"/>
+      <c r="F33" s="141"/>
       <c r="G33" s="141"/>
       <c r="H33" s="141"/>
       <c r="I33" s="141"/>
@@ -4971,223 +4856,50 @@
       <c r="K33" s="141"/>
       <c r="L33" s="141"/>
       <c r="M33" s="141"/>
-      <c r="N33" s="143"/>
-    </row>
-    <row r="34" s="140" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="141"/>
-      <c r="C34" s="141"/>
-      <c r="D34" s="141"/>
-      <c r="E34" s="141"/>
-      <c r="F34" s="142"/>
-      <c r="G34" s="141"/>
-      <c r="H34" s="141"/>
-      <c r="I34" s="141"/>
-      <c r="J34" s="141"/>
-      <c r="K34" s="141"/>
-      <c r="L34" s="141"/>
-      <c r="M34" s="141"/>
-      <c r="N34" s="143"/>
-    </row>
-    <row r="35" s="140" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="141"/>
-      <c r="C35" s="141"/>
-      <c r="D35" s="141"/>
-      <c r="E35" s="141"/>
-      <c r="F35" s="142"/>
-      <c r="G35" s="141"/>
-      <c r="H35" s="141"/>
-      <c r="I35" s="141"/>
-      <c r="J35" s="141"/>
-      <c r="K35" s="141"/>
-      <c r="L35" s="141"/>
-      <c r="M35" s="141"/>
-      <c r="N35" s="143"/>
-    </row>
-    <row r="36" s="140" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="141"/>
-      <c r="C36" s="141"/>
-      <c r="D36" s="141"/>
-      <c r="E36" s="141"/>
-      <c r="F36" s="142"/>
-      <c r="G36" s="141"/>
-      <c r="H36" s="141"/>
-      <c r="I36" s="141"/>
-      <c r="J36" s="141"/>
-      <c r="K36" s="141"/>
-      <c r="L36" s="141"/>
-      <c r="M36" s="141"/>
-      <c r="N36" s="143"/>
-    </row>
-    <row r="37" s="140" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="141"/>
-      <c r="C37" s="141"/>
-      <c r="D37" s="141"/>
-      <c r="E37" s="141"/>
-      <c r="F37" s="142"/>
-      <c r="G37" s="141"/>
-      <c r="H37" s="141"/>
-      <c r="I37" s="141"/>
-      <c r="J37" s="141"/>
-      <c r="K37" s="141"/>
-      <c r="L37" s="141"/>
-      <c r="M37" s="141"/>
-      <c r="N37" s="143"/>
-    </row>
-    <row r="38" s="140" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="141"/>
-      <c r="C38" s="141"/>
-      <c r="D38" s="141"/>
-      <c r="E38" s="141"/>
-      <c r="F38" s="142"/>
-      <c r="G38" s="141"/>
-      <c r="H38" s="141"/>
-      <c r="I38" s="141"/>
-      <c r="J38" s="141"/>
-      <c r="K38" s="141"/>
-      <c r="L38" s="141"/>
-      <c r="M38" s="141"/>
-      <c r="N38" s="143"/>
-    </row>
-    <row r="39" s="140" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="141"/>
-      <c r="C39" s="141"/>
-      <c r="D39" s="141"/>
-      <c r="E39" s="141"/>
-      <c r="F39" s="142"/>
-      <c r="G39" s="141"/>
-      <c r="H39" s="141"/>
-      <c r="I39" s="141"/>
-      <c r="J39" s="141"/>
-      <c r="K39" s="141"/>
-      <c r="L39" s="141"/>
-      <c r="M39" s="141"/>
-      <c r="N39" s="143"/>
-    </row>
-    <row r="40" s="140" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="141"/>
-      <c r="C40" s="141"/>
-      <c r="D40" s="141"/>
-      <c r="E40" s="141"/>
-      <c r="F40" s="142"/>
-      <c r="G40" s="141"/>
-      <c r="H40" s="141"/>
-      <c r="I40" s="141"/>
-      <c r="J40" s="141"/>
-      <c r="K40" s="141"/>
-      <c r="L40" s="141"/>
-      <c r="M40" s="141"/>
-      <c r="N40" s="143"/>
-    </row>
-    <row r="42" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="144" t="s">
-        <v>143</v>
-      </c>
-      <c r="C42" s="144"/>
-      <c r="D42" s="144"/>
-      <c r="E42" s="144"/>
-      <c r="F42" s="144"/>
-      <c r="G42" s="144"/>
-      <c r="H42" s="144"/>
-      <c r="I42" s="144"/>
-      <c r="J42" s="144"/>
-      <c r="K42" s="144"/>
-      <c r="L42" s="144"/>
-      <c r="M42" s="144"/>
-      <c r="N42" s="144"/>
-    </row>
-    <row r="43" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="144"/>
-      <c r="C43" s="144"/>
-      <c r="D43" s="144"/>
-      <c r="E43" s="144"/>
-      <c r="F43" s="144"/>
-      <c r="G43" s="144"/>
-      <c r="H43" s="144"/>
-      <c r="I43" s="144"/>
-      <c r="J43" s="144"/>
-      <c r="K43" s="144"/>
-      <c r="L43" s="144"/>
-      <c r="M43" s="144"/>
-      <c r="N43" s="144"/>
-    </row>
-    <row r="44" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="145" t="s">
+      <c r="N33" s="141"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G38" s="142"/>
+    </row>
+    <row r="41" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="141" t="s">
         <v>144</v>
       </c>
-      <c r="C44" s="145"/>
-      <c r="D44" s="145"/>
-      <c r="E44" s="145"/>
-      <c r="F44" s="145"/>
-      <c r="G44" s="145"/>
-      <c r="H44" s="145"/>
-      <c r="I44" s="145"/>
-      <c r="J44" s="145"/>
-      <c r="K44" s="145"/>
-      <c r="L44" s="145"/>
-      <c r="M44" s="145"/>
-      <c r="N44" s="145"/>
-    </row>
-    <row r="45" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="145"/>
-      <c r="C45" s="145"/>
-      <c r="D45" s="145"/>
-      <c r="E45" s="145"/>
-      <c r="F45" s="145"/>
-      <c r="G45" s="145"/>
-      <c r="H45" s="145"/>
-      <c r="I45" s="145"/>
-      <c r="J45" s="145"/>
-      <c r="K45" s="145"/>
-      <c r="L45" s="145"/>
-      <c r="M45" s="145"/>
-      <c r="N45" s="145"/>
-    </row>
-    <row r="46" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="146" t="s">
+      <c r="C41" s="141"/>
+      <c r="D41" s="141"/>
+      <c r="H41" s="141" t="s">
+        <v>144</v>
+      </c>
+      <c r="I41" s="141"/>
+      <c r="J41" s="141"/>
+    </row>
+    <row r="42" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="141" t="s">
         <v>145</v>
       </c>
-      <c r="C46" s="146"/>
-      <c r="D46" s="146"/>
-      <c r="E46" s="146"/>
-      <c r="F46" s="146"/>
-      <c r="G46" s="146"/>
-      <c r="H46" s="146"/>
-      <c r="I46" s="146"/>
-      <c r="J46" s="146"/>
-      <c r="K46" s="146"/>
-      <c r="L46" s="146"/>
-      <c r="M46" s="146"/>
-      <c r="N46" s="146"/>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G51" s="147"/>
-    </row>
-    <row r="54" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="146" t="s">
-        <v>146</v>
-      </c>
-      <c r="C54" s="146"/>
-      <c r="D54" s="146"/>
-      <c r="H54" s="146" t="s">
-        <v>146</v>
-      </c>
-      <c r="I54" s="146"/>
-      <c r="J54" s="146"/>
-    </row>
-    <row r="55" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="146" t="s">
-        <v>147</v>
-      </c>
-      <c r="C55" s="146"/>
-      <c r="D55" s="146"/>
-      <c r="H55" s="146" t="s">
-        <v>147</v>
-      </c>
-      <c r="I55" s="146"/>
-      <c r="J55" s="146"/>
-    </row>
+      <c r="C42" s="141"/>
+      <c r="D42" s="141"/>
+      <c r="H42" s="141" t="s">
+        <v>145</v>
+      </c>
+      <c r="I42" s="141"/>
+      <c r="J42" s="141"/>
+    </row>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="74">
+  <mergeCells count="35">
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="B4:N4"/>
     <mergeCell ref="B8:N8"/>
@@ -5221,47 +4933,8 @@
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="I27:K27"/>
     <mergeCell ref="L27:M27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I38:K38"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="I39:K39"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="B42:N43"/>
-    <mergeCell ref="B44:N45"/>
+    <mergeCell ref="B29:N30"/>
+    <mergeCell ref="B31:N32"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
HREOS-12585 modificada ficha comercial segun requerimientos
</commit_message>
<xml_diff>
--- a/rem-web/src/main/webapp/plantillas/plugin/GenerarFichaComercialBbva/FichaComercialReport.xlsx
+++ b/rem-web/src/main/webapp/plantillas/plugin/GenerarFichaComercialBbva/FichaComercialReport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Oferta BBVA" sheetId="1" state="visible" r:id="rId2"/>
@@ -815,7 +815,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -862,12 +862,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFE7E6E6"/>
         <bgColor rgb="FFEDEDED"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -1230,7 +1224,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1282,7 +1276,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1545,6 +1539,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="171" fontId="18" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1613,6 +1611,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="171" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1621,14 +1623,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="9" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1653,79 +1647,79 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="10" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="9" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="10" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="10" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="10" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="11" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="10" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="11" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="10" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="10" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="10" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="10" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="10" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1741,19 +1735,19 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1864,9 +1858,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1503720</xdr:colOff>
+      <xdr:colOff>1503360</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
+      <xdr:rowOff>154800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1881,7 +1875,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="533520" y="190440"/>
-          <a:ext cx="1503360" cy="505440"/>
+          <a:ext cx="1503000" cy="505080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1907,9 +1901,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1128600</xdr:colOff>
+      <xdr:colOff>1128240</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>121320</xdr:rowOff>
+      <xdr:rowOff>120960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1924,7 +1918,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="279360" y="190440"/>
-          <a:ext cx="1990800" cy="502200"/>
+          <a:ext cx="1990440" cy="501840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1950,9 +1944,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>37080</xdr:colOff>
+      <xdr:colOff>36720</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>124560</xdr:rowOff>
+      <xdr:rowOff>124200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1967,7 +1961,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="254160" y="190440"/>
-          <a:ext cx="1911240" cy="505440"/>
+          <a:ext cx="1910880" cy="505080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1993,9 +1987,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>18000</xdr:colOff>
+      <xdr:colOff>17640</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>124560</xdr:rowOff>
+      <xdr:rowOff>124200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2010,7 +2004,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="317520" y="190440"/>
-          <a:ext cx="1892160" cy="505440"/>
+          <a:ext cx="1891800" cy="505080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2072,7 +2066,7 @@
   </sheetPr>
   <dimension ref="B2:M74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -2919,15 +2913,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B4:AH22"/>
+  <dimension ref="B1:AH21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <pane xSplit="3" ySplit="0" topLeftCell="Y1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AD19" activeCellId="0" sqref="AD19"/>
+      <selection pane="topRight" activeCell="AF16" activeCellId="0" sqref="AF16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.7"/>
@@ -2945,50 +2939,66 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="25.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="20" style="0" width="12.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="20" style="0" width="12.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="90" width="12.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="12.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="11.71"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AD1" s="0"/>
+      <c r="AE1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AD2" s="0"/>
+      <c r="AE2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AD3" s="0"/>
+      <c r="AE3" s="0"/>
+    </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V4" s="90"/>
+      <c r="V4" s="91"/>
+      <c r="AD4" s="0"/>
+      <c r="AE4" s="0"/>
     </row>
     <row r="5" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91"/>
-      <c r="K5" s="91"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="91"/>
-      <c r="N5" s="91"/>
-      <c r="O5" s="91"/>
-      <c r="P5" s="91"/>
-      <c r="Q5" s="91"/>
-      <c r="R5" s="91"/>
-      <c r="S5" s="91"/>
-      <c r="T5" s="93"/>
-      <c r="U5" s="93"/>
-      <c r="V5" s="93"/>
-      <c r="W5" s="93"/>
-      <c r="X5" s="93"/>
-      <c r="Y5" s="93"/>
-      <c r="Z5" s="93"/>
-      <c r="AA5" s="93"/>
-      <c r="AB5" s="94"/>
-      <c r="AC5" s="93"/>
-      <c r="AD5" s="93"/>
-      <c r="AE5" s="93"/>
-      <c r="AF5" s="93"/>
-      <c r="AG5" s="93"/>
-      <c r="AH5" s="91"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="93"/>
+      <c r="M5" s="92"/>
+      <c r="N5" s="92"/>
+      <c r="O5" s="92"/>
+      <c r="P5" s="92"/>
+      <c r="Q5" s="92"/>
+      <c r="R5" s="92"/>
+      <c r="S5" s="92"/>
+      <c r="T5" s="94"/>
+      <c r="U5" s="94"/>
+      <c r="V5" s="94"/>
+      <c r="W5" s="94"/>
+      <c r="X5" s="94"/>
+      <c r="Y5" s="94"/>
+      <c r="Z5" s="94"/>
+      <c r="AA5" s="94"/>
+      <c r="AB5" s="95"/>
+      <c r="AC5" s="94"/>
+      <c r="AD5" s="94"/>
+      <c r="AE5" s="94"/>
+      <c r="AF5" s="94"/>
+      <c r="AG5" s="94"/>
+      <c r="AH5" s="92"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="89"/>
@@ -3013,599 +3023,600 @@
       <c r="Y6" s="89"/>
       <c r="Z6" s="89"/>
       <c r="AA6" s="89"/>
+      <c r="AD6" s="0"/>
+      <c r="AE6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="95" t="s">
+      <c r="B7" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="96" t="s">
+      <c r="C7" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="96" t="s">
+      <c r="D7" s="97" t="s">
         <v>86</v>
       </c>
-      <c r="E7" s="96" t="s">
+      <c r="E7" s="97" t="s">
         <v>87</v>
       </c>
-      <c r="F7" s="96" t="s">
+      <c r="F7" s="97" t="s">
         <v>88</v>
       </c>
-      <c r="G7" s="95" t="s">
+      <c r="G7" s="96" t="s">
         <v>89</v>
       </c>
-      <c r="H7" s="97" t="s">
+      <c r="H7" s="98" t="s">
         <v>90</v>
       </c>
-      <c r="I7" s="97" t="s">
+      <c r="I7" s="98" t="s">
         <v>91</v>
       </c>
-      <c r="J7" s="97" t="s">
+      <c r="J7" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="K7" s="98" t="s">
+      <c r="K7" s="99" t="s">
         <v>93</v>
       </c>
-      <c r="L7" s="96" t="s">
+      <c r="L7" s="97" t="s">
         <v>94</v>
       </c>
-      <c r="M7" s="97" t="s">
+      <c r="M7" s="98" t="s">
         <v>95</v>
       </c>
-      <c r="N7" s="96" t="s">
+      <c r="N7" s="97" t="s">
         <v>96</v>
       </c>
-      <c r="O7" s="97" t="s">
+      <c r="O7" s="98" t="s">
         <v>58</v>
       </c>
-      <c r="P7" s="96" t="s">
+      <c r="P7" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="Q7" s="97" t="s">
+      <c r="Q7" s="98" t="s">
         <v>97</v>
       </c>
-      <c r="R7" s="95" t="s">
+      <c r="R7" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="S7" s="97" t="s">
+      <c r="S7" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="T7" s="96" t="s">
+      <c r="T7" s="97" t="s">
         <v>34</v>
       </c>
-      <c r="U7" s="96" t="s">
+      <c r="U7" s="97" t="s">
         <v>99</v>
       </c>
-      <c r="V7" s="96" t="s">
+      <c r="V7" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="W7" s="96" t="s">
+      <c r="W7" s="97" t="s">
         <v>36</v>
       </c>
-      <c r="X7" s="96" t="s">
+      <c r="X7" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="Y7" s="96" t="s">
+      <c r="Y7" s="97" t="s">
         <v>100</v>
       </c>
-      <c r="Z7" s="96" t="s">
+      <c r="Z7" s="97" t="s">
         <v>101</v>
       </c>
-      <c r="AA7" s="96" t="s">
+      <c r="AA7" s="97" t="s">
         <v>102</v>
       </c>
-      <c r="AB7" s="96" t="s">
+      <c r="AB7" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="AC7" s="96" t="s">
+      <c r="AC7" s="97" t="s">
         <v>103</v>
       </c>
-      <c r="AD7" s="96" t="s">
+      <c r="AD7" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="AE7" s="96" t="s">
+      <c r="AE7" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="AF7" s="96" t="s">
+      <c r="AF7" s="97" t="s">
         <v>104</v>
       </c>
-      <c r="AG7" s="99" t="s">
+      <c r="AG7" s="100" t="s">
         <v>105</v>
       </c>
-      <c r="AH7" s="95" t="s">
+      <c r="AH7" s="96" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="8" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="100"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="101"/>
-      <c r="G8" s="100"/>
-      <c r="H8" s="102"/>
-      <c r="I8" s="102"/>
-      <c r="J8" s="100"/>
-      <c r="K8" s="102"/>
-      <c r="L8" s="103"/>
-      <c r="M8" s="102"/>
-      <c r="N8" s="101"/>
-      <c r="O8" s="102"/>
-      <c r="P8" s="101"/>
-      <c r="Q8" s="102"/>
-      <c r="R8" s="102"/>
-      <c r="S8" s="102"/>
-      <c r="T8" s="104"/>
-      <c r="U8" s="104"/>
-      <c r="V8" s="105"/>
-      <c r="W8" s="104"/>
-      <c r="X8" s="105"/>
-      <c r="Y8" s="104"/>
-      <c r="Z8" s="104"/>
-      <c r="AA8" s="104"/>
-      <c r="AB8" s="103"/>
-      <c r="AC8" s="106"/>
-      <c r="AD8" s="105"/>
-      <c r="AE8" s="105"/>
-      <c r="AF8" s="105"/>
-      <c r="AG8" s="107"/>
-      <c r="AH8" s="100"/>
+      <c r="B8" s="101"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="101"/>
+      <c r="K8" s="103"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="103"/>
+      <c r="N8" s="102"/>
+      <c r="O8" s="103"/>
+      <c r="P8" s="102"/>
+      <c r="Q8" s="103"/>
+      <c r="R8" s="103"/>
+      <c r="S8" s="103"/>
+      <c r="T8" s="105"/>
+      <c r="U8" s="105"/>
+      <c r="V8" s="106"/>
+      <c r="W8" s="105"/>
+      <c r="X8" s="106"/>
+      <c r="Y8" s="105"/>
+      <c r="Z8" s="105"/>
+      <c r="AA8" s="105"/>
+      <c r="AB8" s="104"/>
+      <c r="AC8" s="107"/>
+      <c r="AD8" s="108"/>
+      <c r="AE8" s="108"/>
+      <c r="AF8" s="106"/>
+      <c r="AG8" s="109"/>
+      <c r="AH8" s="101"/>
     </row>
     <row r="9" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="100"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="100"/>
-      <c r="H9" s="102"/>
-      <c r="I9" s="102"/>
-      <c r="J9" s="100"/>
-      <c r="K9" s="102"/>
-      <c r="L9" s="103"/>
-      <c r="M9" s="102"/>
-      <c r="N9" s="101"/>
-      <c r="O9" s="102"/>
-      <c r="P9" s="101"/>
-      <c r="Q9" s="102"/>
-      <c r="R9" s="102"/>
-      <c r="S9" s="102"/>
-      <c r="T9" s="104"/>
-      <c r="U9" s="104"/>
-      <c r="V9" s="105"/>
-      <c r="W9" s="104"/>
-      <c r="X9" s="105"/>
-      <c r="Y9" s="104"/>
-      <c r="Z9" s="104"/>
-      <c r="AA9" s="104"/>
-      <c r="AB9" s="103"/>
-      <c r="AC9" s="106"/>
-      <c r="AD9" s="105"/>
-      <c r="AE9" s="105"/>
-      <c r="AF9" s="105"/>
-      <c r="AG9" s="107"/>
-      <c r="AH9" s="100"/>
+      <c r="B9" s="101"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="102"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="102"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
+      <c r="J9" s="101"/>
+      <c r="K9" s="103"/>
+      <c r="L9" s="104"/>
+      <c r="M9" s="103"/>
+      <c r="N9" s="102"/>
+      <c r="O9" s="103"/>
+      <c r="P9" s="102"/>
+      <c r="Q9" s="103"/>
+      <c r="R9" s="103"/>
+      <c r="S9" s="103"/>
+      <c r="T9" s="105"/>
+      <c r="U9" s="105"/>
+      <c r="V9" s="106"/>
+      <c r="W9" s="105"/>
+      <c r="X9" s="106"/>
+      <c r="Y9" s="105"/>
+      <c r="Z9" s="105"/>
+      <c r="AA9" s="105"/>
+      <c r="AB9" s="104"/>
+      <c r="AC9" s="107"/>
+      <c r="AD9" s="108"/>
+      <c r="AE9" s="108"/>
+      <c r="AF9" s="106"/>
+      <c r="AG9" s="109"/>
+      <c r="AH9" s="101"/>
     </row>
     <row r="10" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="100"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="100"/>
-      <c r="H10" s="102"/>
-      <c r="I10" s="102"/>
-      <c r="J10" s="100"/>
-      <c r="K10" s="102"/>
-      <c r="L10" s="103"/>
-      <c r="M10" s="102"/>
-      <c r="N10" s="101"/>
-      <c r="O10" s="102"/>
-      <c r="P10" s="101"/>
-      <c r="Q10" s="102"/>
-      <c r="R10" s="102"/>
-      <c r="S10" s="102"/>
-      <c r="T10" s="104"/>
-      <c r="U10" s="104"/>
-      <c r="V10" s="105"/>
-      <c r="W10" s="104"/>
-      <c r="X10" s="105"/>
-      <c r="Y10" s="104"/>
-      <c r="Z10" s="104"/>
-      <c r="AA10" s="104"/>
-      <c r="AB10" s="103"/>
-      <c r="AC10" s="106"/>
-      <c r="AD10" s="105"/>
-      <c r="AE10" s="105"/>
-      <c r="AF10" s="105"/>
-      <c r="AG10" s="107"/>
-      <c r="AH10" s="100"/>
+      <c r="B10" s="101"/>
+      <c r="C10" s="102"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="102"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="101"/>
+      <c r="H10" s="103"/>
+      <c r="I10" s="103"/>
+      <c r="J10" s="101"/>
+      <c r="K10" s="103"/>
+      <c r="L10" s="104"/>
+      <c r="M10" s="103"/>
+      <c r="N10" s="102"/>
+      <c r="O10" s="103"/>
+      <c r="P10" s="102"/>
+      <c r="Q10" s="103"/>
+      <c r="R10" s="103"/>
+      <c r="S10" s="103"/>
+      <c r="T10" s="105"/>
+      <c r="U10" s="105"/>
+      <c r="V10" s="106"/>
+      <c r="W10" s="105"/>
+      <c r="X10" s="106"/>
+      <c r="Y10" s="105"/>
+      <c r="Z10" s="105"/>
+      <c r="AA10" s="105"/>
+      <c r="AB10" s="104"/>
+      <c r="AC10" s="107"/>
+      <c r="AD10" s="108"/>
+      <c r="AE10" s="108"/>
+      <c r="AF10" s="106"/>
+      <c r="AG10" s="109"/>
+      <c r="AH10" s="101"/>
     </row>
     <row r="11" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="100"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="100"/>
-      <c r="H11" s="102"/>
-      <c r="I11" s="102"/>
-      <c r="J11" s="100"/>
-      <c r="K11" s="102"/>
-      <c r="L11" s="103"/>
-      <c r="M11" s="102"/>
-      <c r="N11" s="101"/>
-      <c r="O11" s="102"/>
-      <c r="P11" s="101"/>
-      <c r="Q11" s="102"/>
-      <c r="R11" s="102"/>
-      <c r="S11" s="102"/>
-      <c r="T11" s="104"/>
-      <c r="U11" s="104"/>
-      <c r="V11" s="105"/>
-      <c r="W11" s="104"/>
-      <c r="X11" s="105"/>
-      <c r="Y11" s="104"/>
-      <c r="Z11" s="104"/>
-      <c r="AA11" s="104"/>
-      <c r="AB11" s="103"/>
-      <c r="AC11" s="106"/>
-      <c r="AD11" s="105"/>
-      <c r="AE11" s="105"/>
-      <c r="AF11" s="105"/>
-      <c r="AG11" s="107"/>
-      <c r="AH11" s="100"/>
+      <c r="B11" s="101"/>
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="101"/>
+      <c r="H11" s="103"/>
+      <c r="I11" s="103"/>
+      <c r="J11" s="101"/>
+      <c r="K11" s="103"/>
+      <c r="L11" s="104"/>
+      <c r="M11" s="103"/>
+      <c r="N11" s="102"/>
+      <c r="O11" s="103"/>
+      <c r="P11" s="102"/>
+      <c r="Q11" s="103"/>
+      <c r="R11" s="103"/>
+      <c r="S11" s="103"/>
+      <c r="T11" s="105"/>
+      <c r="U11" s="105"/>
+      <c r="V11" s="106"/>
+      <c r="W11" s="105"/>
+      <c r="X11" s="106"/>
+      <c r="Y11" s="105"/>
+      <c r="Z11" s="105"/>
+      <c r="AA11" s="105"/>
+      <c r="AB11" s="104"/>
+      <c r="AC11" s="107"/>
+      <c r="AD11" s="108"/>
+      <c r="AE11" s="108"/>
+      <c r="AF11" s="106"/>
+      <c r="AG11" s="109"/>
+      <c r="AH11" s="101"/>
     </row>
     <row r="12" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="100"/>
-      <c r="C12" s="101"/>
-      <c r="D12" s="101"/>
-      <c r="E12" s="101"/>
-      <c r="F12" s="101"/>
-      <c r="G12" s="100"/>
-      <c r="H12" s="102"/>
-      <c r="I12" s="102"/>
-      <c r="J12" s="100"/>
-      <c r="K12" s="102"/>
-      <c r="L12" s="103"/>
-      <c r="M12" s="102"/>
-      <c r="N12" s="101"/>
-      <c r="O12" s="102"/>
-      <c r="P12" s="101"/>
-      <c r="Q12" s="102"/>
-      <c r="R12" s="102"/>
-      <c r="S12" s="102"/>
-      <c r="T12" s="104"/>
-      <c r="U12" s="104"/>
-      <c r="V12" s="105"/>
-      <c r="W12" s="104"/>
-      <c r="X12" s="105"/>
-      <c r="Y12" s="104"/>
-      <c r="Z12" s="104"/>
-      <c r="AA12" s="104"/>
-      <c r="AB12" s="103"/>
-      <c r="AC12" s="106"/>
-      <c r="AD12" s="105"/>
-      <c r="AE12" s="105"/>
-      <c r="AF12" s="105"/>
-      <c r="AG12" s="107"/>
-      <c r="AH12" s="100"/>
+      <c r="B12" s="101"/>
+      <c r="C12" s="102"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="102"/>
+      <c r="G12" s="101"/>
+      <c r="H12" s="103"/>
+      <c r="I12" s="103"/>
+      <c r="J12" s="101"/>
+      <c r="K12" s="103"/>
+      <c r="L12" s="104"/>
+      <c r="M12" s="103"/>
+      <c r="N12" s="102"/>
+      <c r="O12" s="103"/>
+      <c r="P12" s="102"/>
+      <c r="Q12" s="103"/>
+      <c r="R12" s="103"/>
+      <c r="S12" s="103"/>
+      <c r="T12" s="105"/>
+      <c r="U12" s="105"/>
+      <c r="V12" s="106"/>
+      <c r="W12" s="105"/>
+      <c r="X12" s="106"/>
+      <c r="Y12" s="105"/>
+      <c r="Z12" s="105"/>
+      <c r="AA12" s="105"/>
+      <c r="AB12" s="104"/>
+      <c r="AC12" s="107"/>
+      <c r="AD12" s="108"/>
+      <c r="AE12" s="108"/>
+      <c r="AF12" s="106"/>
+      <c r="AG12" s="109"/>
+      <c r="AH12" s="101"/>
     </row>
     <row r="13" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="100"/>
-      <c r="C13" s="101"/>
-      <c r="D13" s="101"/>
-      <c r="E13" s="101"/>
-      <c r="F13" s="101"/>
-      <c r="G13" s="100"/>
-      <c r="H13" s="102"/>
-      <c r="I13" s="102"/>
-      <c r="J13" s="100"/>
-      <c r="K13" s="102"/>
-      <c r="L13" s="103"/>
-      <c r="M13" s="102"/>
-      <c r="N13" s="101"/>
-      <c r="O13" s="102"/>
-      <c r="P13" s="101"/>
-      <c r="Q13" s="102"/>
-      <c r="R13" s="102"/>
-      <c r="S13" s="102"/>
-      <c r="T13" s="104"/>
-      <c r="U13" s="104"/>
-      <c r="V13" s="105"/>
-      <c r="W13" s="104"/>
-      <c r="X13" s="105"/>
-      <c r="Y13" s="104"/>
-      <c r="Z13" s="104"/>
-      <c r="AA13" s="104"/>
-      <c r="AB13" s="103"/>
-      <c r="AC13" s="106"/>
-      <c r="AD13" s="105"/>
-      <c r="AE13" s="105"/>
-      <c r="AF13" s="105"/>
-      <c r="AG13" s="107"/>
-      <c r="AH13" s="100"/>
+      <c r="B13" s="101"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="102"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="102"/>
+      <c r="G13" s="101"/>
+      <c r="H13" s="103"/>
+      <c r="I13" s="103"/>
+      <c r="J13" s="101"/>
+      <c r="K13" s="103"/>
+      <c r="L13" s="104"/>
+      <c r="M13" s="103"/>
+      <c r="N13" s="102"/>
+      <c r="O13" s="103"/>
+      <c r="P13" s="102"/>
+      <c r="Q13" s="103"/>
+      <c r="R13" s="103"/>
+      <c r="S13" s="103"/>
+      <c r="T13" s="105"/>
+      <c r="U13" s="105"/>
+      <c r="V13" s="106"/>
+      <c r="W13" s="105"/>
+      <c r="X13" s="106"/>
+      <c r="Y13" s="105"/>
+      <c r="Z13" s="105"/>
+      <c r="AA13" s="105"/>
+      <c r="AB13" s="104"/>
+      <c r="AC13" s="107"/>
+      <c r="AD13" s="108"/>
+      <c r="AE13" s="108"/>
+      <c r="AF13" s="106"/>
+      <c r="AG13" s="109"/>
+      <c r="AH13" s="101"/>
     </row>
     <row r="14" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="100"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="101"/>
-      <c r="F14" s="101"/>
-      <c r="G14" s="100"/>
-      <c r="H14" s="102"/>
-      <c r="I14" s="102"/>
-      <c r="J14" s="100"/>
-      <c r="K14" s="102"/>
-      <c r="L14" s="103"/>
-      <c r="M14" s="102"/>
-      <c r="N14" s="101"/>
-      <c r="O14" s="102"/>
-      <c r="P14" s="101"/>
-      <c r="Q14" s="102"/>
-      <c r="R14" s="102"/>
-      <c r="S14" s="102"/>
-      <c r="T14" s="104"/>
-      <c r="U14" s="104"/>
-      <c r="V14" s="105"/>
-      <c r="W14" s="104"/>
-      <c r="X14" s="105"/>
-      <c r="Y14" s="104"/>
-      <c r="Z14" s="104"/>
-      <c r="AA14" s="104"/>
-      <c r="AB14" s="103"/>
-      <c r="AC14" s="106"/>
-      <c r="AD14" s="105"/>
-      <c r="AE14" s="105"/>
-      <c r="AF14" s="105"/>
-      <c r="AG14" s="107"/>
-      <c r="AH14" s="100"/>
+      <c r="B14" s="101"/>
+      <c r="C14" s="102"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="101"/>
+      <c r="H14" s="103"/>
+      <c r="I14" s="103"/>
+      <c r="J14" s="101"/>
+      <c r="K14" s="103"/>
+      <c r="L14" s="104"/>
+      <c r="M14" s="103"/>
+      <c r="N14" s="102"/>
+      <c r="O14" s="103"/>
+      <c r="P14" s="102"/>
+      <c r="Q14" s="103"/>
+      <c r="R14" s="103"/>
+      <c r="S14" s="103"/>
+      <c r="T14" s="105"/>
+      <c r="U14" s="105"/>
+      <c r="V14" s="106"/>
+      <c r="W14" s="105"/>
+      <c r="X14" s="106"/>
+      <c r="Y14" s="105"/>
+      <c r="Z14" s="105"/>
+      <c r="AA14" s="105"/>
+      <c r="AB14" s="104"/>
+      <c r="AC14" s="107"/>
+      <c r="AD14" s="108"/>
+      <c r="AE14" s="108"/>
+      <c r="AF14" s="106"/>
+      <c r="AG14" s="109"/>
+      <c r="AH14" s="101"/>
     </row>
     <row r="15" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="100"/>
-      <c r="C15" s="101"/>
-      <c r="D15" s="101"/>
-      <c r="E15" s="101"/>
-      <c r="F15" s="101"/>
-      <c r="G15" s="100"/>
-      <c r="H15" s="102"/>
-      <c r="I15" s="102"/>
-      <c r="J15" s="100"/>
-      <c r="K15" s="102"/>
-      <c r="L15" s="103"/>
-      <c r="M15" s="102"/>
-      <c r="N15" s="101"/>
-      <c r="O15" s="102"/>
-      <c r="P15" s="101"/>
-      <c r="Q15" s="102"/>
-      <c r="R15" s="102"/>
-      <c r="S15" s="102"/>
-      <c r="T15" s="104"/>
-      <c r="U15" s="104"/>
-      <c r="V15" s="105"/>
-      <c r="W15" s="104"/>
-      <c r="X15" s="105"/>
-      <c r="Y15" s="104"/>
-      <c r="Z15" s="104"/>
-      <c r="AA15" s="104"/>
-      <c r="AB15" s="103"/>
-      <c r="AC15" s="106"/>
-      <c r="AD15" s="105"/>
-      <c r="AE15" s="105"/>
-      <c r="AF15" s="105"/>
-      <c r="AG15" s="107"/>
-      <c r="AH15" s="100"/>
+      <c r="B15" s="101"/>
+      <c r="C15" s="102"/>
+      <c r="D15" s="102"/>
+      <c r="E15" s="102"/>
+      <c r="F15" s="102"/>
+      <c r="G15" s="101"/>
+      <c r="H15" s="103"/>
+      <c r="I15" s="103"/>
+      <c r="J15" s="101"/>
+      <c r="K15" s="103"/>
+      <c r="L15" s="104"/>
+      <c r="M15" s="103"/>
+      <c r="N15" s="102"/>
+      <c r="O15" s="103"/>
+      <c r="P15" s="102"/>
+      <c r="Q15" s="103"/>
+      <c r="R15" s="103"/>
+      <c r="S15" s="103"/>
+      <c r="T15" s="105"/>
+      <c r="U15" s="105"/>
+      <c r="V15" s="106"/>
+      <c r="W15" s="105"/>
+      <c r="X15" s="106"/>
+      <c r="Y15" s="105"/>
+      <c r="Z15" s="105"/>
+      <c r="AA15" s="105"/>
+      <c r="AB15" s="104"/>
+      <c r="AC15" s="107"/>
+      <c r="AD15" s="108"/>
+      <c r="AE15" s="108"/>
+      <c r="AF15" s="106"/>
+      <c r="AG15" s="109"/>
+      <c r="AH15" s="101"/>
     </row>
     <row r="16" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="100"/>
-      <c r="C16" s="101"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="100"/>
-      <c r="H16" s="102"/>
-      <c r="I16" s="102"/>
-      <c r="J16" s="100"/>
-      <c r="K16" s="102"/>
-      <c r="L16" s="103"/>
-      <c r="M16" s="102"/>
-      <c r="N16" s="101"/>
-      <c r="O16" s="102"/>
-      <c r="P16" s="101"/>
-      <c r="Q16" s="102"/>
-      <c r="R16" s="102"/>
-      <c r="S16" s="102"/>
-      <c r="T16" s="104"/>
-      <c r="U16" s="104"/>
-      <c r="V16" s="105"/>
-      <c r="W16" s="104"/>
-      <c r="X16" s="105"/>
-      <c r="Y16" s="104"/>
-      <c r="Z16" s="104"/>
-      <c r="AA16" s="104"/>
-      <c r="AB16" s="103"/>
-      <c r="AC16" s="106"/>
-      <c r="AD16" s="105"/>
-      <c r="AE16" s="105"/>
-      <c r="AF16" s="105"/>
-      <c r="AG16" s="107"/>
-      <c r="AH16" s="100"/>
+      <c r="B16" s="101"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="101"/>
+      <c r="H16" s="103"/>
+      <c r="I16" s="103"/>
+      <c r="J16" s="101"/>
+      <c r="K16" s="103"/>
+      <c r="L16" s="104"/>
+      <c r="M16" s="103"/>
+      <c r="N16" s="102"/>
+      <c r="O16" s="103"/>
+      <c r="P16" s="102"/>
+      <c r="Q16" s="103"/>
+      <c r="R16" s="103"/>
+      <c r="S16" s="103"/>
+      <c r="T16" s="105"/>
+      <c r="U16" s="105"/>
+      <c r="V16" s="106"/>
+      <c r="W16" s="105"/>
+      <c r="X16" s="106"/>
+      <c r="Y16" s="105"/>
+      <c r="Z16" s="105"/>
+      <c r="AA16" s="105"/>
+      <c r="AB16" s="104"/>
+      <c r="AC16" s="107"/>
+      <c r="AD16" s="108"/>
+      <c r="AE16" s="108"/>
+      <c r="AF16" s="106"/>
+      <c r="AG16" s="109"/>
+      <c r="AH16" s="101"/>
     </row>
     <row r="17" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="100"/>
-      <c r="C17" s="101"/>
-      <c r="D17" s="101"/>
-      <c r="E17" s="101"/>
-      <c r="F17" s="101"/>
-      <c r="G17" s="100"/>
-      <c r="H17" s="102"/>
-      <c r="I17" s="102"/>
-      <c r="J17" s="100"/>
-      <c r="K17" s="102"/>
-      <c r="L17" s="103"/>
-      <c r="M17" s="102"/>
-      <c r="N17" s="101"/>
-      <c r="O17" s="102"/>
-      <c r="P17" s="101"/>
-      <c r="Q17" s="102"/>
-      <c r="R17" s="102"/>
-      <c r="S17" s="102"/>
-      <c r="T17" s="104"/>
-      <c r="U17" s="104"/>
-      <c r="V17" s="105"/>
-      <c r="W17" s="104"/>
-      <c r="X17" s="105"/>
-      <c r="Y17" s="104"/>
-      <c r="Z17" s="104"/>
-      <c r="AA17" s="104"/>
-      <c r="AB17" s="103"/>
-      <c r="AC17" s="106"/>
-      <c r="AD17" s="105"/>
-      <c r="AE17" s="105"/>
-      <c r="AF17" s="105"/>
-      <c r="AG17" s="107"/>
-      <c r="AH17" s="100"/>
+      <c r="B17" s="101"/>
+      <c r="C17" s="102"/>
+      <c r="D17" s="102"/>
+      <c r="E17" s="102"/>
+      <c r="F17" s="102"/>
+      <c r="G17" s="101"/>
+      <c r="H17" s="103"/>
+      <c r="I17" s="103"/>
+      <c r="J17" s="101"/>
+      <c r="K17" s="103"/>
+      <c r="L17" s="104"/>
+      <c r="M17" s="103"/>
+      <c r="N17" s="102"/>
+      <c r="O17" s="103"/>
+      <c r="P17" s="102"/>
+      <c r="Q17" s="103"/>
+      <c r="R17" s="103"/>
+      <c r="S17" s="103"/>
+      <c r="T17" s="105"/>
+      <c r="U17" s="105"/>
+      <c r="V17" s="106"/>
+      <c r="W17" s="105"/>
+      <c r="X17" s="106"/>
+      <c r="Y17" s="105"/>
+      <c r="Z17" s="105"/>
+      <c r="AA17" s="105"/>
+      <c r="AB17" s="104"/>
+      <c r="AC17" s="107"/>
+      <c r="AD17" s="108"/>
+      <c r="AE17" s="108"/>
+      <c r="AF17" s="106"/>
+      <c r="AG17" s="109"/>
+      <c r="AH17" s="101"/>
     </row>
     <row r="18" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="100"/>
-      <c r="C18" s="101"/>
-      <c r="D18" s="101"/>
-      <c r="E18" s="101"/>
-      <c r="F18" s="101"/>
-      <c r="G18" s="100"/>
-      <c r="H18" s="102"/>
-      <c r="I18" s="102"/>
-      <c r="J18" s="100"/>
-      <c r="K18" s="102"/>
-      <c r="L18" s="103"/>
-      <c r="M18" s="102"/>
-      <c r="N18" s="101"/>
-      <c r="O18" s="102"/>
-      <c r="P18" s="101"/>
-      <c r="Q18" s="102"/>
-      <c r="R18" s="102"/>
-      <c r="S18" s="102"/>
-      <c r="T18" s="104"/>
-      <c r="U18" s="104"/>
-      <c r="V18" s="105"/>
-      <c r="W18" s="104"/>
-      <c r="X18" s="105"/>
-      <c r="Y18" s="104"/>
-      <c r="Z18" s="104"/>
-      <c r="AA18" s="104"/>
-      <c r="AB18" s="103"/>
-      <c r="AC18" s="106"/>
-      <c r="AD18" s="105"/>
-      <c r="AE18" s="105"/>
-      <c r="AF18" s="105"/>
-      <c r="AG18" s="107"/>
-      <c r="AH18" s="100"/>
+      <c r="B18" s="101"/>
+      <c r="C18" s="102"/>
+      <c r="D18" s="102"/>
+      <c r="E18" s="102"/>
+      <c r="F18" s="102"/>
+      <c r="G18" s="101"/>
+      <c r="H18" s="103"/>
+      <c r="I18" s="103"/>
+      <c r="J18" s="101"/>
+      <c r="K18" s="103"/>
+      <c r="L18" s="104"/>
+      <c r="M18" s="103"/>
+      <c r="N18" s="102"/>
+      <c r="O18" s="103"/>
+      <c r="P18" s="102"/>
+      <c r="Q18" s="103"/>
+      <c r="R18" s="103"/>
+      <c r="S18" s="103"/>
+      <c r="T18" s="105"/>
+      <c r="U18" s="105"/>
+      <c r="V18" s="106"/>
+      <c r="W18" s="105"/>
+      <c r="X18" s="106"/>
+      <c r="Y18" s="105"/>
+      <c r="Z18" s="105"/>
+      <c r="AA18" s="105"/>
+      <c r="AB18" s="104"/>
+      <c r="AC18" s="107"/>
+      <c r="AD18" s="108"/>
+      <c r="AE18" s="108"/>
+      <c r="AF18" s="106"/>
+      <c r="AG18" s="109"/>
+      <c r="AH18" s="101"/>
     </row>
     <row r="19" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="100"/>
-      <c r="C19" s="101"/>
-      <c r="D19" s="101"/>
-      <c r="E19" s="101"/>
-      <c r="F19" s="101"/>
-      <c r="G19" s="100"/>
-      <c r="H19" s="102"/>
-      <c r="I19" s="102"/>
-      <c r="J19" s="100"/>
-      <c r="K19" s="102"/>
-      <c r="L19" s="103"/>
-      <c r="M19" s="102"/>
-      <c r="N19" s="101"/>
-      <c r="O19" s="102"/>
-      <c r="P19" s="101"/>
-      <c r="Q19" s="102"/>
-      <c r="R19" s="102"/>
-      <c r="S19" s="102"/>
-      <c r="T19" s="104"/>
-      <c r="U19" s="104"/>
-      <c r="V19" s="105"/>
-      <c r="W19" s="104"/>
-      <c r="X19" s="105"/>
-      <c r="Y19" s="104"/>
-      <c r="Z19" s="104"/>
-      <c r="AA19" s="104"/>
-      <c r="AB19" s="103"/>
-      <c r="AC19" s="106"/>
-      <c r="AD19" s="105"/>
-      <c r="AE19" s="105"/>
-      <c r="AF19" s="105"/>
-      <c r="AG19" s="107"/>
-      <c r="AH19" s="100"/>
+      <c r="B19" s="101"/>
+      <c r="C19" s="102"/>
+      <c r="D19" s="102"/>
+      <c r="E19" s="102"/>
+      <c r="F19" s="102"/>
+      <c r="G19" s="101"/>
+      <c r="H19" s="103"/>
+      <c r="I19" s="103"/>
+      <c r="J19" s="101"/>
+      <c r="K19" s="103"/>
+      <c r="L19" s="104"/>
+      <c r="M19" s="103"/>
+      <c r="N19" s="102"/>
+      <c r="O19" s="103"/>
+      <c r="P19" s="102"/>
+      <c r="Q19" s="103"/>
+      <c r="R19" s="103"/>
+      <c r="S19" s="103"/>
+      <c r="T19" s="105"/>
+      <c r="U19" s="105"/>
+      <c r="V19" s="106"/>
+      <c r="W19" s="105"/>
+      <c r="X19" s="106"/>
+      <c r="Y19" s="105"/>
+      <c r="Z19" s="105"/>
+      <c r="AA19" s="105"/>
+      <c r="AB19" s="104"/>
+      <c r="AC19" s="107"/>
+      <c r="AD19" s="108"/>
+      <c r="AE19" s="108"/>
+      <c r="AF19" s="106"/>
+      <c r="AG19" s="109"/>
+      <c r="AH19" s="101"/>
     </row>
     <row r="20" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="100"/>
-      <c r="C20" s="101"/>
-      <c r="D20" s="101"/>
-      <c r="E20" s="101"/>
-      <c r="F20" s="101"/>
-      <c r="G20" s="100"/>
-      <c r="H20" s="102"/>
-      <c r="I20" s="102"/>
-      <c r="J20" s="100"/>
-      <c r="K20" s="102"/>
-      <c r="L20" s="103"/>
-      <c r="M20" s="102"/>
-      <c r="N20" s="101"/>
-      <c r="O20" s="102"/>
-      <c r="P20" s="101"/>
-      <c r="Q20" s="102"/>
-      <c r="R20" s="102"/>
-      <c r="S20" s="102"/>
-      <c r="T20" s="104"/>
-      <c r="U20" s="104"/>
-      <c r="V20" s="105"/>
-      <c r="W20" s="104"/>
-      <c r="X20" s="105"/>
-      <c r="Y20" s="104"/>
-      <c r="Z20" s="104"/>
-      <c r="AA20" s="104"/>
-      <c r="AB20" s="103"/>
-      <c r="AC20" s="106"/>
-      <c r="AD20" s="105"/>
-      <c r="AE20" s="105"/>
-      <c r="AF20" s="105"/>
-      <c r="AG20" s="107"/>
-      <c r="AH20" s="100"/>
+      <c r="B20" s="101"/>
+      <c r="C20" s="102"/>
+      <c r="D20" s="102"/>
+      <c r="E20" s="102"/>
+      <c r="F20" s="102"/>
+      <c r="G20" s="101"/>
+      <c r="H20" s="103"/>
+      <c r="I20" s="103"/>
+      <c r="J20" s="101"/>
+      <c r="K20" s="103"/>
+      <c r="L20" s="104"/>
+      <c r="M20" s="103"/>
+      <c r="N20" s="102"/>
+      <c r="O20" s="103"/>
+      <c r="P20" s="102"/>
+      <c r="Q20" s="103"/>
+      <c r="R20" s="103"/>
+      <c r="S20" s="103"/>
+      <c r="T20" s="105"/>
+      <c r="U20" s="105"/>
+      <c r="V20" s="106"/>
+      <c r="W20" s="105"/>
+      <c r="X20" s="106"/>
+      <c r="Y20" s="105"/>
+      <c r="Z20" s="105"/>
+      <c r="AA20" s="105"/>
+      <c r="AB20" s="104"/>
+      <c r="AC20" s="107"/>
+      <c r="AD20" s="108"/>
+      <c r="AE20" s="108"/>
+      <c r="AF20" s="106"/>
+      <c r="AG20" s="109"/>
+      <c r="AH20" s="101"/>
     </row>
     <row r="21" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="100"/>
-      <c r="C21" s="101"/>
-      <c r="D21" s="101"/>
-      <c r="E21" s="101"/>
-      <c r="F21" s="101"/>
-      <c r="G21" s="100"/>
-      <c r="H21" s="102"/>
-      <c r="I21" s="102"/>
-      <c r="J21" s="100"/>
-      <c r="K21" s="102"/>
-      <c r="L21" s="103"/>
-      <c r="M21" s="102"/>
-      <c r="N21" s="101"/>
-      <c r="O21" s="102"/>
-      <c r="P21" s="101"/>
-      <c r="Q21" s="102"/>
-      <c r="R21" s="102"/>
-      <c r="S21" s="102"/>
-      <c r="T21" s="104"/>
-      <c r="U21" s="104"/>
-      <c r="V21" s="105"/>
-      <c r="W21" s="104"/>
-      <c r="X21" s="105"/>
-      <c r="Y21" s="104"/>
-      <c r="Z21" s="104"/>
-      <c r="AA21" s="104"/>
-      <c r="AB21" s="103"/>
-      <c r="AC21" s="106"/>
-      <c r="AD21" s="105"/>
-      <c r="AE21" s="105"/>
-      <c r="AF21" s="105"/>
-      <c r="AG21" s="107"/>
-      <c r="AH21" s="100"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B21" s="101"/>
+      <c r="C21" s="102"/>
+      <c r="D21" s="102"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="102"/>
+      <c r="G21" s="101"/>
+      <c r="H21" s="103"/>
+      <c r="I21" s="103"/>
+      <c r="J21" s="101"/>
+      <c r="K21" s="103"/>
+      <c r="L21" s="104"/>
+      <c r="M21" s="103"/>
+      <c r="N21" s="102"/>
+      <c r="O21" s="103"/>
+      <c r="P21" s="102"/>
+      <c r="Q21" s="103"/>
+      <c r="R21" s="103"/>
+      <c r="S21" s="103"/>
+      <c r="T21" s="105"/>
+      <c r="U21" s="105"/>
+      <c r="V21" s="106"/>
+      <c r="W21" s="105"/>
+      <c r="X21" s="106"/>
+      <c r="Y21" s="105"/>
+      <c r="Z21" s="105"/>
+      <c r="AA21" s="105"/>
+      <c r="AB21" s="104"/>
+      <c r="AC21" s="107"/>
+      <c r="AD21" s="108"/>
+      <c r="AE21" s="108"/>
+      <c r="AF21" s="106"/>
+      <c r="AG21" s="109"/>
+      <c r="AH21" s="101"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B8:B21">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
@@ -3633,10 +3644,10 @@
   </sheetPr>
   <dimension ref="B1:T21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topRight" activeCell="O7" activeCellId="0" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3657,27 +3668,27 @@
       <c r="Q4" s="89"/>
     </row>
     <row r="5" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="92" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91"/>
-      <c r="K5" s="91"/>
-      <c r="L5" s="91"/>
-      <c r="M5" s="91"/>
-      <c r="N5" s="91"/>
-      <c r="O5" s="91"/>
-      <c r="P5" s="91"/>
-      <c r="Q5" s="91"/>
-      <c r="R5" s="91"/>
-      <c r="S5" s="91"/>
-      <c r="T5" s="91"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="92"/>
+      <c r="M5" s="92"/>
+      <c r="N5" s="92"/>
+      <c r="O5" s="92"/>
+      <c r="P5" s="92"/>
+      <c r="Q5" s="92"/>
+      <c r="R5" s="92"/>
+      <c r="S5" s="92"/>
+      <c r="T5" s="92"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="89"/>
@@ -3700,61 +3711,61 @@
       <c r="T6" s="89"/>
     </row>
     <row r="7" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="95" t="s">
+      <c r="B7" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="96" t="s">
+      <c r="C7" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="108" t="s">
+      <c r="D7" s="110" t="s">
         <v>86</v>
       </c>
-      <c r="E7" s="108" t="s">
+      <c r="E7" s="110" t="s">
         <v>87</v>
       </c>
-      <c r="F7" s="96" t="s">
+      <c r="F7" s="97" t="s">
         <v>88</v>
       </c>
-      <c r="G7" s="95" t="s">
+      <c r="G7" s="96" t="s">
         <v>89</v>
       </c>
-      <c r="H7" s="97" t="s">
+      <c r="H7" s="98" t="s">
         <v>108</v>
       </c>
-      <c r="I7" s="109" t="s">
+      <c r="I7" s="98" t="s">
         <v>109</v>
       </c>
-      <c r="J7" s="97" t="s">
+      <c r="J7" s="98" t="s">
         <v>110</v>
       </c>
-      <c r="K7" s="97" t="s">
+      <c r="K7" s="98" t="s">
         <v>111</v>
       </c>
-      <c r="L7" s="97" t="s">
+      <c r="L7" s="98" t="s">
         <v>112</v>
       </c>
-      <c r="M7" s="98" t="s">
+      <c r="M7" s="99" t="s">
         <v>113</v>
       </c>
-      <c r="N7" s="97" t="s">
+      <c r="N7" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="O7" s="110" t="s">
+      <c r="O7" s="97" t="s">
         <v>115</v>
       </c>
-      <c r="P7" s="97" t="s">
+      <c r="P7" s="98" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="96" t="s">
+      <c r="Q7" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="R7" s="97" t="s">
+      <c r="R7" s="98" t="s">
         <v>97</v>
       </c>
-      <c r="S7" s="95" t="s">
+      <c r="S7" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="T7" s="97" t="s">
+      <c r="T7" s="98" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4076,7 +4087,7 @@
   </sheetPr>
   <dimension ref="B1:M22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
HREOS-13357  version-2.25.3-rem  Cambios ficha comercial
</commit_message>
<xml_diff>
--- a/rem-web/src/main/webapp/plantillas/plugin/GenerarFichaComercialBbva/FichaComercialReport.xlsx
+++ b/rem-web/src/main/webapp/plantillas/plugin/GenerarFichaComercialBbva/FichaComercialReport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Oferta BBVA" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="141">
   <si>
     <t xml:space="preserve">ID OFERTA:</t>
   </si>
@@ -412,9 +412,6 @@
   </si>
   <si>
     <t xml:space="preserve">HISTÓRICO DE OFERTAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esta Hoja estará vacía para que el GM incluya las fotografías que considere, REM generará la hoja vacía pero SI tiene que estar</t>
   </si>
   <si>
     <t xml:space="preserve">AUTORIZACIÓN ESPECIAL PARA LA VENTA DE INMUEBLES</t>
@@ -1852,9 +1849,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1501560</xdr:colOff>
+      <xdr:colOff>1500840</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:rowOff>152280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1869,7 +1866,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="533520" y="190440"/>
-          <a:ext cx="1501200" cy="503280"/>
+          <a:ext cx="1500480" cy="502560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1895,9 +1892,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1126440</xdr:colOff>
+      <xdr:colOff>1125720</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>119160</xdr:rowOff>
+      <xdr:rowOff>118440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1912,7 +1909,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="279360" y="190440"/>
-          <a:ext cx="1988640" cy="500040"/>
+          <a:ext cx="1987920" cy="499320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1938,9 +1935,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>34920</xdr:colOff>
+      <xdr:colOff>34200</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>122400</xdr:rowOff>
+      <xdr:rowOff>121680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1955,7 +1952,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="254160" y="190440"/>
-          <a:ext cx="1909080" cy="503280"/>
+          <a:ext cx="1908360" cy="502560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1981,9 +1978,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>15840</xdr:colOff>
+      <xdr:colOff>15120</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>122400</xdr:rowOff>
+      <xdr:rowOff>121680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1998,7 +1995,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="317520" y="190440"/>
-          <a:ext cx="1890000" cy="503280"/>
+          <a:ext cx="1889280" cy="502560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2060,8 +2057,8 @@
   </sheetPr>
   <dimension ref="B2:M74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2929,7 +2926,7 @@
   </sheetPr>
   <dimension ref="B1:AH150"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="0" topLeftCell="Y1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="AA5" activeCellId="0" sqref="AA5"/>
@@ -5660,15 +5657,13 @@
   <dimension ref="B3:I12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="117" t="s">
-        <v>113</v>
-      </c>
+      <c r="B3" s="117"/>
       <c r="C3" s="117"/>
       <c r="D3" s="117"/>
       <c r="E3" s="117"/>
@@ -5828,7 +5823,7 @@
     <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="119"/>
       <c r="B2" s="120" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" s="120"/>
       <c r="D2" s="120"/>
@@ -5862,7 +5857,7 @@
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="119"/>
       <c r="B4" s="121" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C4" s="121"/>
       <c r="D4" s="121"/>
@@ -5896,7 +5891,7 @@
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="119"/>
       <c r="B6" s="122" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6" s="122"/>
       <c r="D6" s="122"/>
@@ -5930,7 +5925,7 @@
     <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="119"/>
       <c r="B8" s="121" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" s="121"/>
       <c r="D8" s="121"/>
@@ -5964,7 +5959,7 @@
     <row r="10" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="119"/>
       <c r="B10" s="123" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C10" s="123"/>
       <c r="D10" s="123"/>
@@ -5998,7 +5993,7 @@
     <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="119"/>
       <c r="B12" s="121" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C12" s="121"/>
       <c r="D12" s="121"/>
@@ -6032,7 +6027,7 @@
     <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="119"/>
       <c r="B14" s="122" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" s="122"/>
       <c r="D14" s="122"/>
@@ -6065,37 +6060,37 @@
     </row>
     <row r="16" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="125" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C16" s="125"/>
       <c r="D16" s="125" t="s">
+        <v>121</v>
+      </c>
+      <c r="E16" s="125" t="s">
         <v>122</v>
-      </c>
-      <c r="E16" s="125" t="s">
-        <v>123</v>
       </c>
       <c r="F16" s="125"/>
       <c r="G16" s="126" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" s="126" t="s">
         <v>124</v>
       </c>
-      <c r="H16" s="126" t="s">
+      <c r="I16" s="125" t="s">
         <v>125</v>
       </c>
-      <c r="I16" s="125" t="s">
+      <c r="J16" s="125" t="s">
         <v>126</v>
       </c>
-      <c r="J16" s="125" t="s">
+      <c r="K16" s="126" t="s">
         <v>127</v>
       </c>
-      <c r="K16" s="126" t="s">
+      <c r="L16" s="125" t="s">
         <v>128</v>
-      </c>
-      <c r="L16" s="125" t="s">
-        <v>129</v>
       </c>
       <c r="M16" s="125"/>
       <c r="N16" s="125" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6190,7 +6185,7 @@
     </row>
     <row r="24" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="132" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C24" s="132"/>
       <c r="D24" s="132"/>
@@ -6207,19 +6202,19 @@
     </row>
     <row r="26" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="133" t="s">
+        <v>131</v>
+      </c>
+      <c r="C26" s="133" t="s">
         <v>132</v>
       </c>
-      <c r="C26" s="133" t="s">
+      <c r="D26" s="133" t="s">
         <v>133</v>
-      </c>
-      <c r="D26" s="133" t="s">
-        <v>134</v>
       </c>
       <c r="E26" s="133" t="s">
         <v>85</v>
       </c>
       <c r="F26" s="133" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G26" s="134" t="s">
         <v>54</v>
@@ -6235,7 +6230,7 @@
       </c>
       <c r="M26" s="134"/>
       <c r="N26" s="134" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O26" s="135"/>
     </row>
@@ -6256,7 +6251,7 @@
     </row>
     <row r="29" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="140" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C29" s="140"/>
       <c r="D29" s="140"/>
@@ -6288,7 +6283,7 @@
     </row>
     <row r="31" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="141" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C31" s="141"/>
       <c r="D31" s="141"/>
@@ -6320,7 +6315,7 @@
     </row>
     <row r="33" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="142" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C33" s="142"/>
       <c r="D33" s="142"/>
@@ -6340,24 +6335,24 @@
     </row>
     <row r="41" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="142" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C41" s="142"/>
       <c r="D41" s="142"/>
       <c r="H41" s="142" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I41" s="142"/>
       <c r="J41" s="142"/>
     </row>
     <row r="42" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="142" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C42" s="142"/>
       <c r="D42" s="142"/>
       <c r="H42" s="142" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I42" s="142"/>
       <c r="J42" s="142"/>

</xml_diff>

<commit_message>
HREOS-13357 Modificaciones ficha comercial
</commit_message>
<xml_diff>
--- a/rem-web/src/main/webapp/plantillas/plugin/GenerarFichaComercialBbva/FichaComercialReport.xlsx
+++ b/rem-web/src/main/webapp/plantillas/plugin/GenerarFichaComercialBbva/FichaComercialReport.xlsx
@@ -114,7 +114,7 @@
     <t xml:space="preserve">Fecha modif. PVP</t>
   </si>
   <si>
-    <t xml:space="preserve">Dto delegado</t>
+    <t xml:space="preserve">Descuento</t>
   </si>
   <si>
     <t xml:space="preserve">Precio Comité (€)</t>
@@ -1849,9 +1849,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1500840</xdr:colOff>
+      <xdr:colOff>1500480</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1866,7 +1866,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="533520" y="190440"/>
-          <a:ext cx="1500480" cy="502560"/>
+          <a:ext cx="1500120" cy="502200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1892,9 +1892,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1125720</xdr:colOff>
+      <xdr:colOff>1125360</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>118440</xdr:rowOff>
+      <xdr:rowOff>118080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1909,7 +1909,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="279360" y="190440"/>
-          <a:ext cx="1987920" cy="499320"/>
+          <a:ext cx="1987560" cy="498960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1935,9 +1935,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>34200</xdr:colOff>
+      <xdr:colOff>33840</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>121680</xdr:rowOff>
+      <xdr:rowOff>121320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1952,7 +1952,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="254160" y="190440"/>
-          <a:ext cx="1908360" cy="502560"/>
+          <a:ext cx="1908000" cy="502200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1978,9 +1978,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>15120</xdr:colOff>
+      <xdr:colOff>14760</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>121680</xdr:rowOff>
+      <xdr:rowOff>121320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1995,7 +1995,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="317520" y="190440"/>
-          <a:ext cx="1889280" cy="502560"/>
+          <a:ext cx="1888920" cy="502200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2057,8 +2057,8 @@
   </sheetPr>
   <dimension ref="B2:M74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L31" activeCellId="0" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>